<commit_message>
Update results for Undocumented Model Elements
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="37">
   <si>
     <t>Mediastore</t>
   </si>
@@ -125,6 +125,12 @@
   </si>
   <si>
     <t>DELTA All/No</t>
+  </si>
+  <si>
+    <t>#ModelElements</t>
+  </si>
+  <si>
+    <t>TN</t>
   </si>
 </sst>
 </file>
@@ -231,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -245,6 +251,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -527,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:X76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C33" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="N62" sqref="N62"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1355,77 +1362,77 @@
       </c>
       <c r="D15" s="2">
         <f>(Info!$B$2*Results!D5+Info!$B$3*Results!D6+Info!$B$4*Results!D7+Info!$B$5*Results!D8+Info!$B$6*Results!D9+Info!$B$7*Results!D10+Info!$B$8*Results!D11+Info!$B$9*Results!D12+Info!$B$10*Results!D13)/SUM(Info!$B$2:C$10)</f>
-        <v>0.80624000000000007</v>
+        <v>0.63445036319612591</v>
       </c>
       <c r="E15" s="2">
         <f>(Info!$B$2*Results!E5+Info!$B$3*Results!E6+Info!$B$4*Results!E7+Info!$B$5*Results!E8+Info!$B$6*Results!E9+Info!$B$7*Results!E10+Info!$B$8*Results!E11+Info!$B$9*Results!E12+Info!$B$10*Results!E13)/SUM(Info!$B$2:D$10)</f>
-        <v>0.79448307692307707</v>
+        <v>0.6251985472154965</v>
       </c>
       <c r="F15" s="2">
         <f>(Info!$B$2*Results!F5+Info!$B$3*Results!F6+Info!$B$4*Results!F7+Info!$B$5*Results!F8+Info!$B$6*Results!F9+Info!$B$7*Results!F10+Info!$B$8*Results!F11+Info!$B$9*Results!F12+Info!$B$10*Results!F13)/SUM(Info!$B$2:E$10)</f>
-        <v>0.98108615384615372</v>
+        <v>0.77204116222760277</v>
       </c>
       <c r="G15" s="2">
         <f>(Info!$B$2*Results!G5+Info!$B$3*Results!G6+Info!$B$4*Results!G7+Info!$B$5*Results!G8+Info!$B$6*Results!G9+Info!$B$7*Results!G10+Info!$B$8*Results!G11+Info!$B$9*Results!G12+Info!$B$10*Results!G13)/SUM(Info!$B$2:F$10)</f>
-        <v>0.98913538461538464</v>
+        <v>0.77837530266343824</v>
       </c>
       <c r="H15" s="2">
         <f>(Info!$B$2*Results!H5+Info!$B$3*Results!H6+Info!$B$4*Results!H7+Info!$B$5*Results!H8+Info!$B$6*Results!H9+Info!$B$7*Results!H10+Info!$B$8*Results!H11+Info!$B$9*Results!H12+Info!$B$10*Results!H13)/SUM(Info!$B$2:G$10)</f>
-        <v>0.79310153846153841</v>
+        <v>0.62411138014527845</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>19</v>
       </c>
       <c r="K15" s="2">
         <f>(Info!$B$2*Results!K5+Info!$B$3*Results!K6+Info!$B$4*Results!K7+Info!$B$5*Results!K8+Info!$B$6*Results!K9+Info!$B$7*Results!K10+Info!$B$8*Results!K11+Info!$B$9*Results!K12+Info!$B$10*Results!K13)/SUM(Info!$B$2:J$10)</f>
-        <v>0.79843076923076928</v>
+        <v>0.62830508474576274</v>
       </c>
       <c r="L15" s="2">
         <f>(Info!$B$2*Results!L5+Info!$B$3*Results!L6+Info!$B$4*Results!L7+Info!$B$5*Results!L8+Info!$B$6*Results!L9+Info!$B$7*Results!L10+Info!$B$8*Results!L11+Info!$B$9*Results!L12+Info!$B$10*Results!L13)/SUM(Info!$B$2:K$10)</f>
-        <v>0.36732615384615386</v>
+        <v>0.28905811138014526</v>
       </c>
       <c r="M15" s="2">
         <f>(Info!$B$2*Results!M5+Info!$B$3*Results!M6+Info!$B$4*Results!M7+Info!$B$5*Results!M8+Info!$B$6*Results!M9+Info!$B$7*Results!M10+Info!$B$8*Results!M11+Info!$B$9*Results!M12+Info!$B$10*Results!M13)/SUM(Info!$B$2:L$10)</f>
-        <v>0.49726461538461525</v>
+        <v>0.39130992736077475</v>
       </c>
       <c r="N15" s="2">
         <f>(Info!$B$2*Results!N5+Info!$B$3*Results!N6+Info!$B$4*Results!N7+Info!$B$5*Results!N8+Info!$B$6*Results!N9+Info!$B$7*Results!N10+Info!$B$8*Results!N11+Info!$B$9*Results!N12+Info!$B$10*Results!N13)/SUM(Info!$B$2:M$10)</f>
-        <v>0.89071999999999996</v>
+        <v>0.70092978208232437</v>
       </c>
       <c r="O15" s="2">
         <f>(Info!$B$2*Results!O5+Info!$B$3*Results!O6+Info!$B$4*Results!O7+Info!$B$5*Results!O8+Info!$B$6*Results!O9+Info!$B$7*Results!O10+Info!$B$8*Results!O11+Info!$B$9*Results!O12+Info!$B$10*Results!O13)/SUM(Info!$B$2:N$10)</f>
-        <v>0.98219692307692286</v>
+        <v>0.77291525423728802</v>
       </c>
       <c r="P15" s="2">
         <f>(Info!$B$2*Results!P5+Info!$B$3*Results!P6+Info!$B$4*Results!P7+Info!$B$5*Results!P8+Info!$B$6*Results!P9+Info!$B$7*Results!P10+Info!$B$8*Results!P11+Info!$B$9*Results!P12+Info!$B$10*Results!P13)/SUM(Info!$B$2:O$10)</f>
-        <v>0.48899999999999993</v>
+        <v>0.38480629539951572</v>
       </c>
       <c r="R15" s="3" t="s">
         <v>19</v>
       </c>
       <c r="S15" s="2">
         <f t="shared" ref="S15" si="9">C15-K15</f>
-        <v>1.5846153846153954E-2</v>
+        <v>0.18597183833116049</v>
       </c>
       <c r="T15" s="2">
         <f t="shared" ref="T15" si="10">D15-L15</f>
-        <v>0.43891384615384621</v>
+        <v>0.34539225181598066</v>
       </c>
       <c r="U15" s="2">
         <f t="shared" ref="U15" si="11">E15-M15</f>
-        <v>0.29721846153846182</v>
+        <v>0.23388861985472176</v>
       </c>
       <c r="V15" s="2">
         <f t="shared" ref="V15" si="12">F15-N15</f>
-        <v>9.0366153846153763E-2</v>
+        <v>7.1111380145278402E-2</v>
       </c>
       <c r="W15" s="2">
         <f t="shared" ref="W15" si="13">G15-O15</f>
-        <v>6.938461538461782E-3</v>
+        <v>5.4600484261502213E-3</v>
       </c>
       <c r="X15" s="2">
         <f t="shared" ref="X15" si="14">H15-P15</f>
-        <v>0.30410153846153848</v>
+        <v>0.23930508474576273</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
@@ -2249,77 +2256,77 @@
       </c>
       <c r="D33" s="2">
         <f>(Info!$B$2*Results!D23+Info!$B$3*Results!D24+Info!$B$4*Results!D25+Info!$B$5*Results!D26+Info!$B$6*Results!D27+Info!$B$7*Results!D28+Info!$B$8*Results!D29+Info!$B$9*Results!D30+Info!$B$10*Results!D31)/SUM(Info!$B$2:C$10)</f>
-        <v>0.63681230769230757</v>
+        <v>0.50112348668280859</v>
       </c>
       <c r="E33" s="2">
         <f>(Info!$B$2*Results!E23+Info!$B$3*Results!E24+Info!$B$4*Results!E25+Info!$B$5*Results!E26+Info!$B$6*Results!E27+Info!$B$7*Results!E28+Info!$B$8*Results!E29+Info!$B$9*Results!E30+Info!$B$10*Results!E31)/SUM(Info!$B$2:D$10)</f>
-        <v>0.33547384615384618</v>
+        <v>0.26399273607748186</v>
       </c>
       <c r="F33" s="2">
         <f>(Info!$B$2*Results!F23+Info!$B$3*Results!F24+Info!$B$4*Results!F25+Info!$B$5*Results!F26+Info!$B$6*Results!F27+Info!$B$7*Results!F28+Info!$B$8*Results!F29+Info!$B$9*Results!F30+Info!$B$10*Results!F31)/SUM(Info!$B$2:E$10)</f>
-        <v>0.76057846153846154</v>
+        <v>0.59851815980629541</v>
       </c>
       <c r="G33" s="2">
         <f>(Info!$B$2*Results!G23+Info!$B$3*Results!G24+Info!$B$4*Results!G25+Info!$B$5*Results!G26+Info!$B$6*Results!G27+Info!$B$7*Results!G28+Info!$B$8*Results!G29+Info!$B$9*Results!G30+Info!$B$10*Results!H31)/SUM(Info!$B$2:F$10)</f>
-        <v>0.74934769230769227</v>
+        <v>0.58968038740920092</v>
       </c>
       <c r="H33" s="2">
         <f>(Info!$B$2*Results!H23+Info!$B$3*Results!H24+Info!$B$4*Results!H25+Info!$B$5*Results!H26+Info!$B$6*Results!H27+Info!$B$7*Results!H28+Info!$B$8*Results!H29+Info!$B$9*Results!H30+Info!$B$10*Results!G31)/SUM(Info!$B$2:G$10)</f>
-        <v>0.33149846153846152</v>
+        <v>0.260864406779661</v>
       </c>
       <c r="J33" s="3" t="s">
         <v>19</v>
       </c>
       <c r="K33" s="2">
         <f>(Info!$B$2*Results!K23+Info!$B$3*Results!K24+Info!$B$4*Results!K25+Info!$B$5*Results!K26+Info!$B$6*Results!K27+Info!$B$7*Results!K28+Info!$B$8*Results!K29+Info!$B$9*Results!K30+Info!$B$10*Results!K31)/SUM(Info!$B$2:J$10)</f>
-        <v>8.4766153846153838E-2</v>
+        <v>6.6704600484261495E-2</v>
       </c>
       <c r="L33" s="2">
         <f>(Info!$B$2*Results!L23+Info!$B$3*Results!L24+Info!$B$4*Results!L25+Info!$B$5*Results!L26+Info!$B$6*Results!L27+Info!$B$7*Results!L28+Info!$B$8*Results!L29+Info!$B$9*Results!L30+Info!$B$10*Results!L31)/SUM(Info!$B$2:K$10)</f>
-        <v>0.63386461538461547</v>
+        <v>0.49880387409200977</v>
       </c>
       <c r="M33" s="2">
         <f>(Info!$B$2*Results!M23+Info!$B$3*Results!M24+Info!$B$4*Results!M25+Info!$B$5*Results!M26+Info!$B$6*Results!M27+Info!$B$7*Results!M28+Info!$B$8*Results!M29+Info!$B$9*Results!M30+Info!$B$10*Results!M31)/SUM(Info!$B$2:L$10)</f>
-        <v>0.14035384615384616</v>
+        <v>0.11044794188861987</v>
       </c>
       <c r="N33" s="2">
         <f>(Info!$B$2*Results!N23+Info!$B$3*Results!N24+Info!$B$4*Results!N25+Info!$B$5*Results!N26+Info!$B$6*Results!N27+Info!$B$7*Results!N28+Info!$B$8*Results!N29+Info!$B$9*Results!N30+Info!$B$10*Results!N31)/SUM(Info!$B$2:M$10)</f>
-        <v>0.37375384615384621</v>
+        <v>0.29411622276029059</v>
       </c>
       <c r="O33" s="2">
         <f>(Info!$B$2*Results!P23+Info!$B$3*Results!P24+Info!$B$4*Results!P25+Info!$B$5*Results!O26+Info!$B$6*Results!O27+Info!$B$7*Results!O28+Info!$B$8*Results!O29+Info!$B$9*Results!O30+Info!$B$10*Results!O31)/SUM(Info!$B$2:N$10)</f>
-        <v>0.21770461538461541</v>
+        <v>0.17131719128329298</v>
       </c>
       <c r="P33" s="2">
         <f>(Info!$B$2*Results!P23+Info!$B$3*Results!P24+Info!$B$4*Results!P25+Info!$B$5*Results!P26+Info!$B$6*Results!P27+Info!$B$7*Results!P28+Info!$B$8*Results!P29+Info!$B$9*Results!P30+Info!$B$10*Results!P31)/SUM(Info!$B$2:O$10)</f>
-        <v>1.8276923076923076E-2</v>
+        <v>1.4382566585956415E-2</v>
       </c>
       <c r="R33" s="3" t="s">
         <v>19</v>
       </c>
       <c r="S33" s="2">
         <f t="shared" si="20"/>
-        <v>0.30551384615384619</v>
+        <v>0.32357539951573855</v>
       </c>
       <c r="T33" s="2">
         <f t="shared" si="15"/>
-        <v>2.9476923076920958E-3</v>
+        <v>2.3196125907988252E-3</v>
       </c>
       <c r="U33" s="2">
         <f t="shared" si="16"/>
-        <v>0.19512000000000002</v>
+        <v>0.15354479418886199</v>
       </c>
       <c r="V33" s="2">
         <f t="shared" si="17"/>
-        <v>0.38682461538461532</v>
+        <v>0.30440193704600482</v>
       </c>
       <c r="W33" s="2">
         <f t="shared" si="18"/>
-        <v>0.53164307692307688</v>
+        <v>0.41836319612590794</v>
       </c>
       <c r="X33" s="2">
         <f t="shared" si="19"/>
-        <v>0.31322153846153844</v>
+        <v>0.24648184019370459</v>
       </c>
     </row>
     <row r="35" spans="2:24" x14ac:dyDescent="0.25">
@@ -2454,27 +2461,27 @@
         <v>0</v>
       </c>
       <c r="S37" s="2">
-        <f>C51-K$23</f>
+        <f t="shared" ref="S37:X37" si="24">C51-K$23</f>
         <v>1.3000000000000012E-2</v>
       </c>
       <c r="T37" s="2">
-        <f>D51-L$23</f>
+        <f t="shared" si="24"/>
         <v>-6.9000000000000061E-2</v>
       </c>
       <c r="U37" s="2">
-        <f>E51-M$23</f>
+        <f t="shared" si="24"/>
         <v>1.5000000000000013E-2</v>
       </c>
       <c r="V37" s="2">
-        <f>F51-N$23</f>
+        <f t="shared" si="24"/>
         <v>6.5000000000000058E-2</v>
       </c>
       <c r="W37" s="2">
-        <f>G51-O$23</f>
+        <f t="shared" si="24"/>
         <v>7.5000000000000011E-2</v>
       </c>
       <c r="X37" s="2">
-        <f>H51-P$23</f>
+        <f t="shared" si="24"/>
         <v>-2.0000000000000018E-3</v>
       </c>
     </row>
@@ -2504,54 +2511,54 @@
         <v>1</v>
       </c>
       <c r="K38" s="2">
-        <f t="shared" ref="K38:K44" si="24">C24-C38</f>
+        <f t="shared" ref="K38:K44" si="25">C24-C38</f>
         <v>0.64900000000000002</v>
       </c>
       <c r="L38" s="2">
-        <f t="shared" ref="L38:L45" si="25">D24-D38</f>
+        <f t="shared" ref="L38:L45" si="26">D24-D38</f>
         <v>-3.7000000000000033E-2</v>
       </c>
       <c r="M38" s="2">
-        <f t="shared" ref="M38:M45" si="26">E24-E38</f>
+        <f t="shared" ref="M38:M45" si="27">E24-E38</f>
         <v>0.35000000000000003</v>
       </c>
       <c r="N38" s="2">
-        <f t="shared" ref="N38:N45" si="27">F24-F38</f>
+        <f t="shared" ref="N38:N45" si="28">F24-F38</f>
         <v>0.16299999999999992</v>
       </c>
       <c r="O38" s="2">
-        <f t="shared" ref="O38:O45" si="28">G24-G38</f>
+        <f t="shared" ref="O38:O45" si="29">G24-G38</f>
         <v>0.18899999999999995</v>
       </c>
       <c r="P38" s="2">
-        <f t="shared" ref="P38:P45" si="29">H24-H38</f>
+        <f t="shared" ref="P38:P45" si="30">H24-H38</f>
         <v>0.5</v>
       </c>
       <c r="R38" s="3" t="s">
         <v>1</v>
       </c>
       <c r="S38" s="2">
-        <f>C52-K$24</f>
+        <f t="shared" ref="S38:X38" si="31">C52-K$24</f>
         <v>0.11</v>
       </c>
       <c r="T38" s="2">
-        <f>D52-L$24</f>
+        <f t="shared" si="31"/>
         <v>3.7000000000000033E-2</v>
       </c>
       <c r="U38" s="2">
-        <f>E52-M$24</f>
+        <f t="shared" si="31"/>
         <v>0.14300000000000002</v>
       </c>
       <c r="V38" s="2">
-        <f>F52-N$24</f>
+        <f t="shared" si="31"/>
         <v>0.31200000000000006</v>
       </c>
       <c r="W38" s="2">
-        <f>G52-O$24</f>
+        <f t="shared" si="31"/>
         <v>0.35100000000000003</v>
       </c>
       <c r="X38" s="2">
-        <f>H52-P$24</f>
+        <f t="shared" si="31"/>
         <v>0.17799999999999999</v>
       </c>
     </row>
@@ -2581,27 +2588,27 @@
         <v>6</v>
       </c>
       <c r="K39" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="L39" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="M39" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="N39" s="2">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="O39" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="P39" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="R39" s="3" t="s">
@@ -2612,23 +2619,23 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="T39" s="2">
-        <f t="shared" ref="T39:X39" si="30">D39-L$25</f>
+        <f t="shared" ref="T39:X39" si="32">D39-L$25</f>
         <v>0.5</v>
       </c>
       <c r="U39" s="2">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.12300000000000003</v>
       </c>
       <c r="V39" s="2">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>-9.000000000000008E-3</v>
       </c>
       <c r="W39" s="2">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>-8.3000000000000018E-2</v>
       </c>
       <c r="X39" s="2">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.19600000000000001</v>
       </c>
     </row>
@@ -2658,27 +2665,27 @@
         <v>2</v>
       </c>
       <c r="K40" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>6.699999999999999E-2</v>
       </c>
       <c r="L40" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>-2.0000000000000018E-2</v>
       </c>
       <c r="M40" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>9.099999999999997E-2</v>
       </c>
       <c r="N40" s="2">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.11699999999999999</v>
       </c>
       <c r="O40" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.122</v>
       </c>
       <c r="P40" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>9.099999999999997E-2</v>
       </c>
       <c r="R40" s="3" t="s">
@@ -2689,23 +2696,23 @@
         <v>7.8E-2</v>
       </c>
       <c r="T40" s="2">
-        <f t="shared" ref="T40:X40" si="31">D40-L$26</f>
+        <f t="shared" ref="T40:X40" si="33">D40-L$26</f>
         <v>0.18000000000000005</v>
       </c>
       <c r="U40" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.129</v>
       </c>
       <c r="V40" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.435</v>
       </c>
       <c r="W40" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.443</v>
       </c>
       <c r="X40" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.24100000000000002</v>
       </c>
     </row>
@@ -2735,27 +2742,27 @@
         <v>3</v>
       </c>
       <c r="K41" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>2.8000000000000025E-2</v>
       </c>
       <c r="L41" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>-2.200000000000002E-2</v>
       </c>
       <c r="M41" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="N41" s="2">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>3.7000000000000033E-2</v>
       </c>
       <c r="O41" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>3.9000000000000035E-2</v>
       </c>
       <c r="P41" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="R41" s="3" t="s">
@@ -2766,23 +2773,23 @@
         <v>0.10599999999999998</v>
       </c>
       <c r="T41" s="2">
-        <f t="shared" ref="T41:X41" si="32">D41-L$27</f>
+        <f t="shared" ref="T41:X41" si="34">D41-L$27</f>
         <v>0</v>
       </c>
       <c r="U41" s="2">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>0.16600000000000001</v>
       </c>
       <c r="V41" s="2">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>0.57599999999999996</v>
       </c>
       <c r="W41" s="2">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>0.59799999999999998</v>
       </c>
       <c r="X41" s="2">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>0.26700000000000002</v>
       </c>
     </row>
@@ -2812,27 +2819,27 @@
         <v>4</v>
       </c>
       <c r="K42" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.63100000000000001</v>
       </c>
       <c r="L42" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>-9.600000000000003E-2</v>
       </c>
       <c r="M42" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>9.099999999999997E-2</v>
       </c>
       <c r="N42" s="2">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>9.8999999999999977E-2</v>
       </c>
       <c r="O42" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.11299999999999999</v>
       </c>
       <c r="P42" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.27300000000000002</v>
       </c>
       <c r="R42" s="3" t="s">
@@ -2843,23 +2850,23 @@
         <v>0.17499999999999999</v>
       </c>
       <c r="T42" s="2">
-        <f t="shared" ref="T42:X42" si="33">D42-L$28</f>
+        <f t="shared" ref="T42:X42" si="35">D42-L$28</f>
         <v>-9.5999999999999974E-2</v>
       </c>
       <c r="U42" s="2">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0.19700000000000004</v>
       </c>
       <c r="V42" s="2">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0.40299999999999997</v>
       </c>
       <c r="W42" s="2">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0.433</v>
       </c>
       <c r="X42" s="2">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0.21400000000000002</v>
       </c>
     </row>
@@ -2889,27 +2896,27 @@
         <v>5</v>
       </c>
       <c r="K43" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="L43" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="M43" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="N43" s="2">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="O43" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="P43" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="R43" s="3" t="s">
@@ -2920,23 +2927,23 @@
         <v>-2.5000000000000008E-2</v>
       </c>
       <c r="T43" s="2">
-        <f t="shared" ref="T43:X43" si="34">D43-L$29</f>
+        <f t="shared" ref="T43:X43" si="36">D43-L$29</f>
         <v>-0.79499999999999993</v>
       </c>
       <c r="U43" s="2">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>-8.5000000000000006E-2</v>
       </c>
       <c r="V43" s="2">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0.43099999999999994</v>
       </c>
       <c r="W43" s="2">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0.53699999999999992</v>
       </c>
       <c r="X43" s="2">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>-0.109</v>
       </c>
     </row>
@@ -2966,27 +2973,27 @@
         <v>7</v>
       </c>
       <c r="K44" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="L44" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="M44" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="N44" s="2">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="O44" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="P44" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="R44" s="3" t="s">
@@ -2997,23 +3004,23 @@
         <v>0.86099999999999999</v>
       </c>
       <c r="T44" s="2">
-        <f t="shared" ref="T44:X44" si="35">D44-L$30</f>
+        <f t="shared" ref="T44:X44" si="37">D44-L$30</f>
         <v>0.27700000000000002</v>
       </c>
       <c r="U44" s="2">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>0.30300000000000005</v>
       </c>
       <c r="V44" s="2">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>0.35899999999999999</v>
       </c>
       <c r="W44" s="2">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>0.35199999999999998</v>
       </c>
       <c r="X44" s="2">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>0.74399999999999999</v>
       </c>
     </row>
@@ -3047,23 +3054,23 @@
         <v>0</v>
       </c>
       <c r="L45" s="10">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="M45" s="10">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="N45" s="10">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="O45" s="10">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="P45" s="10">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="R45" s="4" t="s">
@@ -3074,23 +3081,23 @@
         <v>3.7000000000000005E-2</v>
       </c>
       <c r="T45" s="10">
-        <f t="shared" ref="T45:X45" si="36">D45-L$31</f>
+        <f t="shared" ref="T45:X45" si="38">D45-L$31</f>
         <v>0</v>
       </c>
       <c r="U45" s="10">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2.2000000000000006E-2</v>
       </c>
       <c r="V45" s="10">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>0.14499999999999999</v>
       </c>
       <c r="W45" s="10">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>0.81699999999999995</v>
       </c>
       <c r="X45" s="10">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>-0.501</v>
       </c>
     </row>
@@ -3103,15 +3110,15 @@
         <v>0.26044444444444448</v>
       </c>
       <c r="D46" s="7">
-        <f t="shared" ref="D46:F46" si="37">SUM(D37:D45)/COUNT(D37:D45)</f>
+        <f t="shared" ref="D46:F46" si="39">SUM(D37:D45)/COUNT(D37:D45)</f>
         <v>0.58966666666666656</v>
       </c>
       <c r="E46" s="7">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>0.26766666666666672</v>
       </c>
       <c r="F46" s="7">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>0.68655555555555559</v>
       </c>
       <c r="G46" s="7">
@@ -3119,34 +3126,34 @@
         <v>0.71144444444444455</v>
       </c>
       <c r="H46" s="7">
-        <f t="shared" ref="H46" si="38">SUM(H37:H45)/COUNT(H37:H45)</f>
+        <f t="shared" ref="H46" si="40">SUM(H37:H45)/COUNT(H37:H45)</f>
         <v>0.19011111111111109</v>
       </c>
       <c r="J46" s="3" t="s">
         <v>18</v>
       </c>
       <c r="K46" s="2">
-        <f t="shared" ref="K46:K47" si="39">C32-C46</f>
+        <f t="shared" ref="K46:K47" si="41">C32-C46</f>
         <v>0.15877777777777774</v>
       </c>
       <c r="L46" s="2">
-        <f t="shared" ref="L46:L47" si="40">D32-D46</f>
+        <f t="shared" ref="L46:L47" si="42">D32-D46</f>
         <v>-2.7111111111111086E-2</v>
       </c>
       <c r="M46" s="2">
-        <f t="shared" ref="M46:M47" si="41">E32-E46</f>
+        <f t="shared" ref="M46:M47" si="43">E32-E46</f>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="N46" s="2">
-        <f t="shared" ref="N46:N47" si="42">F32-F46</f>
+        <f t="shared" ref="N46:N47" si="44">F32-F46</f>
         <v>6.2111111111111117E-2</v>
       </c>
       <c r="O46" s="2">
-        <f t="shared" ref="O46:O47" si="43">G32-G46</f>
+        <f t="shared" ref="O46:O47" si="45">G32-G46</f>
         <v>6.9666666666666544E-2</v>
       </c>
       <c r="P46" s="2">
-        <f t="shared" ref="P46:P47" si="44">H32-H46</f>
+        <f t="shared" ref="P46:P47" si="46">H32-H46</f>
         <v>0.10544444444444448</v>
       </c>
       <c r="R46" s="3" t="s">
@@ -3157,23 +3164,23 @@
         <v>0.16800000000000004</v>
       </c>
       <c r="T46" s="2">
-        <f t="shared" ref="T46:X46" si="45">D46-L$32</f>
+        <f t="shared" ref="T46:X46" si="47">D46-L$32</f>
         <v>3.7777777777776578E-3</v>
       </c>
       <c r="U46" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>0.12288888888888894</v>
       </c>
       <c r="V46" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>0.31455555555555553</v>
       </c>
       <c r="W46" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>0.4057777777777779</v>
       </c>
       <c r="X46" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>0.1482222222222222</v>
       </c>
     </row>
@@ -3187,77 +3194,77 @@
       </c>
       <c r="D47" s="2">
         <f>(Info!$B$2*Results!D51+Info!$B$3*Results!D52+Info!$B$4*Results!D39+Info!$B$5*Results!D40+Info!$B$6*Results!D41+Info!$B$7*Results!D42+Info!$B$8*Results!D43+Info!$B$9*Results!D44+Info!$B$10*Results!D45)/SUM(Info!$B$2:C$10)</f>
-        <v>0.66759384615384609</v>
+        <v>0.52534624697336563</v>
       </c>
       <c r="E47" s="2">
         <f>(Info!$B$2*Results!E51+Info!$B$3*Results!E52+Info!$B$4*Results!E39+Info!$B$5*Results!E40+Info!$B$6*Results!E41+Info!$B$7*Results!E42+Info!$B$8*Results!E43+Info!$B$9*Results!E44+Info!$B$10*Results!E45)/SUM(Info!$B$2:D$10)</f>
-        <v>0.25964000000000004</v>
+        <v>0.20431719128329301</v>
       </c>
       <c r="F47" s="2">
         <f>(Info!$B$2*Results!F51+Info!$B$3*Results!F52+Info!$B$4*Results!F39+Info!$B$5*Results!F40+Info!$B$6*Results!F41+Info!$B$7*Results!F42+Info!$B$8*Results!F43+Info!$B$9*Results!F44+Info!$B$10*Results!F45)/SUM(Info!$B$2:E$10)</f>
-        <v>0.68572923076923065</v>
+        <v>0.53961743341404356</v>
       </c>
       <c r="G47" s="2">
         <f>(Info!$B$2*Results!G51+Info!$B$3*Results!G52+Info!$B$4*Results!G39+Info!$B$5*Results!G40+Info!$B$6*Results!G41+Info!$B$7*Results!G42+Info!$B$8*Results!G43+Info!$B$9*Results!G44+Info!$B$10*Results!H45)/SUM(Info!$B$2:F$10)</f>
-        <v>0.66592615384615372</v>
+        <v>0.52403389830508462</v>
       </c>
       <c r="H47" s="2">
         <f>(Info!$B$2*Results!H51+Info!$B$3*Results!H52+Info!$B$4*Results!H39+Info!$B$5*Results!H40+Info!$B$6*Results!H41+Info!$B$7*Results!H42+Info!$B$8*Results!H43+Info!$B$9*Results!H44+Info!$B$10*Results!G45)/SUM(Info!$B$2:G$10)</f>
-        <v>0.21415692307692311</v>
+        <v>0.1685254237288136</v>
       </c>
       <c r="J47" s="3" t="s">
         <v>19</v>
       </c>
       <c r="K47" s="2">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>0.18119384615384615</v>
       </c>
       <c r="L47" s="2">
-        <f t="shared" si="40"/>
-        <v>-3.0781538461538527E-2</v>
+        <f t="shared" si="42"/>
+        <v>-2.4222760290557033E-2</v>
       </c>
       <c r="M47" s="2">
-        <f t="shared" si="41"/>
-        <v>7.5833846153846141E-2</v>
+        <f t="shared" si="43"/>
+        <v>5.9675544794188851E-2</v>
       </c>
       <c r="N47" s="2">
-        <f t="shared" si="42"/>
-        <v>7.484923076923089E-2</v>
+        <f t="shared" si="44"/>
+        <v>5.8900726392251856E-2</v>
       </c>
       <c r="O47" s="2">
-        <f t="shared" si="43"/>
-        <v>8.3421538461538547E-2</v>
+        <f t="shared" si="45"/>
+        <v>6.5646489104116301E-2</v>
       </c>
       <c r="P47" s="2">
-        <f t="shared" si="44"/>
-        <v>0.11734153846153841</v>
+        <f t="shared" si="46"/>
+        <v>9.2338983050847395E-2</v>
       </c>
       <c r="R47" s="3" t="s">
         <v>19</v>
       </c>
       <c r="S47" s="2">
         <f>C47-K$33</f>
-        <v>0.12432000000000003</v>
+        <v>0.14238155336189237</v>
       </c>
       <c r="T47" s="2">
-        <f t="shared" ref="T47:X47" si="46">D47-L$33</f>
-        <v>3.3729230769230623E-2</v>
+        <f t="shared" ref="T47:X47" si="48">D47-L$33</f>
+        <v>2.6542372881355858E-2</v>
       </c>
       <c r="U47" s="2">
-        <f t="shared" si="46"/>
-        <v>0.11928615384615388</v>
+        <f t="shared" si="48"/>
+        <v>9.3869249394673143E-2</v>
       </c>
       <c r="V47" s="2">
-        <f t="shared" si="46"/>
-        <v>0.31197538461538443</v>
+        <f t="shared" si="48"/>
+        <v>0.24550121065375297</v>
       </c>
       <c r="W47" s="2">
-        <f t="shared" si="46"/>
-        <v>0.44822153846153834</v>
+        <f t="shared" si="48"/>
+        <v>0.35271670702179164</v>
       </c>
       <c r="X47" s="2">
-        <f t="shared" si="46"/>
-        <v>0.19588000000000003</v>
+        <f t="shared" si="48"/>
+        <v>0.15414285714285719</v>
       </c>
     </row>
     <row r="49" spans="2:24" x14ac:dyDescent="0.25">
@@ -3369,23 +3376,23 @@
         <v>5.3999999999999992E-2</v>
       </c>
       <c r="L51" s="2">
-        <f t="shared" ref="L51:P51" si="47">D23-D51</f>
+        <f t="shared" ref="L51:P51" si="49">D23-D51</f>
         <v>-6.899999999999995E-2</v>
       </c>
       <c r="M51" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="N51" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>0.1429999999999999</v>
       </c>
       <c r="O51" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>0.16399999999999992</v>
       </c>
       <c r="P51" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>5.3000000000000019E-2</v>
       </c>
       <c r="R51" s="3" t="s">
@@ -3396,23 +3403,23 @@
         <v>1.3000000000000012E-2</v>
       </c>
       <c r="T51" s="2">
-        <f t="shared" ref="T51:X51" si="48">D51-L$23</f>
+        <f t="shared" ref="T51:X51" si="50">D51-L$23</f>
         <v>-6.9000000000000061E-2</v>
       </c>
       <c r="U51" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>1.5000000000000013E-2</v>
       </c>
       <c r="V51" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>6.5000000000000058E-2</v>
       </c>
       <c r="W51" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>7.5000000000000011E-2</v>
       </c>
       <c r="X51" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>-2.0000000000000018E-3</v>
       </c>
     </row>
@@ -3442,27 +3449,27 @@
         <v>1</v>
       </c>
       <c r="K52" s="2">
-        <f t="shared" ref="K52:K61" si="49">C24-C52</f>
+        <f t="shared" ref="K52:K61" si="51">C24-C52</f>
         <v>0.73599999999999999</v>
       </c>
       <c r="L52" s="2">
-        <f t="shared" ref="L52:L61" si="50">D24-D52</f>
+        <f t="shared" ref="L52:L61" si="52">D24-D52</f>
         <v>-3.7000000000000033E-2</v>
       </c>
       <c r="M52" s="2">
-        <f t="shared" ref="M52:M61" si="51">E24-E52</f>
+        <f t="shared" ref="M52:M61" si="53">E24-E52</f>
         <v>0.443</v>
       </c>
       <c r="N52" s="2">
-        <f t="shared" ref="N52:N61" si="52">F24-F52</f>
+        <f t="shared" ref="N52:N61" si="54">F24-F52</f>
         <v>0.27699999999999991</v>
       </c>
       <c r="O52" s="2">
-        <f t="shared" ref="O52:O61" si="53">G24-G52</f>
+        <f t="shared" ref="O52:O61" si="55">G24-G52</f>
         <v>0.31799999999999995</v>
       </c>
       <c r="P52" s="2">
-        <f t="shared" ref="P52:P61" si="54">H24-H52</f>
+        <f t="shared" ref="P52:P61" si="56">H24-H52</f>
         <v>0.60500000000000009</v>
       </c>
       <c r="R52" s="3" t="s">
@@ -3473,23 +3480,23 @@
         <v>0.11</v>
       </c>
       <c r="T52" s="2">
-        <f t="shared" ref="T52:X52" si="55">D52-L$24</f>
+        <f t="shared" ref="T52:X52" si="57">D52-L$24</f>
         <v>3.7000000000000033E-2</v>
       </c>
       <c r="U52" s="2">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>0.14300000000000002</v>
       </c>
       <c r="V52" s="2">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>0.31200000000000006</v>
       </c>
       <c r="W52" s="2">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>0.35100000000000003</v>
       </c>
       <c r="X52" s="2">
-        <f t="shared" si="55"/>
+        <f t="shared" si="57"/>
         <v>0.17799999999999999</v>
       </c>
     </row>
@@ -3519,54 +3526,54 @@
         <v>6</v>
       </c>
       <c r="K53" s="2">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="L53" s="2">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="M53" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="N53" s="2">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="O53" s="2">
-        <f t="shared" si="53"/>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="P53" s="2">
-        <f t="shared" si="54"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="R53" s="3" t="s">
         <v>6</v>
       </c>
       <c r="S53" s="2">
-        <f>C53-K$25</f>
+        <f t="shared" ref="S53:X53" si="58">C53-K$25</f>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="T53" s="2">
-        <f>D53-L$25</f>
+        <f t="shared" si="58"/>
         <v>0.5</v>
       </c>
       <c r="U53" s="2">
-        <f>E53-M$25</f>
+        <f t="shared" si="58"/>
         <v>0.12300000000000003</v>
       </c>
       <c r="V53" s="2">
-        <f>F53-N$25</f>
+        <f t="shared" si="58"/>
         <v>-9.000000000000008E-3</v>
       </c>
       <c r="W53" s="2">
-        <f>G53-O$25</f>
+        <f t="shared" si="58"/>
         <v>-8.3000000000000018E-2</v>
       </c>
       <c r="X53" s="2">
-        <f>H53-P$25</f>
+        <f t="shared" si="58"/>
         <v>0.19600000000000001</v>
       </c>
     </row>
@@ -3596,27 +3603,27 @@
         <v>2</v>
       </c>
       <c r="K54" s="2">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>6.7999999999999991E-2</v>
       </c>
       <c r="L54" s="2">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>-7.999999999999996E-2</v>
       </c>
       <c r="M54" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>9.1999999999999971E-2</v>
       </c>
       <c r="N54" s="2">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0.13</v>
       </c>
       <c r="O54" s="2">
-        <f t="shared" si="53"/>
+        <f t="shared" si="55"/>
         <v>0.13700000000000001</v>
       </c>
       <c r="P54" s="2">
-        <f t="shared" si="54"/>
+        <f t="shared" si="56"/>
         <v>7.6999999999999985E-2</v>
       </c>
       <c r="R54" s="3" t="s">
@@ -3627,23 +3634,23 @@
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="T54" s="2">
-        <f t="shared" ref="T54" si="56">D54-L$26</f>
+        <f t="shared" ref="T54" si="59">D54-L$26</f>
         <v>0.24</v>
       </c>
       <c r="U54" s="2">
-        <f t="shared" ref="U54" si="57">E54-M$26</f>
+        <f t="shared" ref="U54" si="60">E54-M$26</f>
         <v>0.128</v>
       </c>
       <c r="V54" s="2">
-        <f t="shared" ref="V54" si="58">F54-N$26</f>
+        <f t="shared" ref="V54" si="61">F54-N$26</f>
         <v>0.42199999999999999</v>
       </c>
       <c r="W54" s="2">
-        <f t="shared" ref="W54" si="59">G54-O$26</f>
+        <f t="shared" ref="W54" si="62">G54-O$26</f>
         <v>0.42799999999999999</v>
       </c>
       <c r="X54" s="2">
-        <f t="shared" ref="X54" si="60">H54-P$26</f>
+        <f t="shared" ref="X54" si="63">H54-P$26</f>
         <v>0.255</v>
       </c>
     </row>
@@ -3673,27 +3680,27 @@
         <v>3</v>
       </c>
       <c r="K55" s="2">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>3.6000000000000004E-2</v>
       </c>
       <c r="L55" s="2">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>-0.10899999999999999</v>
       </c>
       <c r="M55" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>4.0000000000000008E-2</v>
       </c>
       <c r="N55" s="2">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>7.1999999999999953E-2</v>
       </c>
       <c r="O55" s="2">
-        <f t="shared" si="53"/>
+        <f t="shared" si="55"/>
         <v>7.8999999999999959E-2</v>
       </c>
       <c r="P55" s="2">
-        <f t="shared" si="54"/>
+        <f t="shared" si="56"/>
         <v>0.03</v>
       </c>
       <c r="R55" s="3" t="s">
@@ -3704,23 +3711,23 @@
         <v>9.8000000000000004E-2</v>
       </c>
       <c r="T55" s="2">
-        <f t="shared" ref="T55" si="61">D55-L$27</f>
+        <f t="shared" ref="T55" si="64">D55-L$27</f>
         <v>8.6999999999999966E-2</v>
       </c>
       <c r="U55" s="2">
-        <f t="shared" ref="U55" si="62">E55-M$27</f>
+        <f t="shared" ref="U55" si="65">E55-M$27</f>
         <v>0.159</v>
       </c>
       <c r="V55" s="2">
-        <f t="shared" ref="V55" si="63">F55-N$27</f>
+        <f t="shared" ref="V55" si="66">F55-N$27</f>
         <v>0.54100000000000004</v>
       </c>
       <c r="W55" s="2">
-        <f t="shared" ref="W55" si="64">G55-O$27</f>
+        <f t="shared" ref="W55" si="67">G55-O$27</f>
         <v>0.55800000000000005</v>
       </c>
       <c r="X55" s="2">
-        <f t="shared" ref="X55" si="65">H55-P$27</f>
+        <f t="shared" ref="X55" si="68">H55-P$27</f>
         <v>0.27</v>
       </c>
     </row>
@@ -3750,27 +3757,27 @@
         <v>4</v>
       </c>
       <c r="K56" s="2">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>0.68500000000000005</v>
       </c>
       <c r="L56" s="2">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>-9.600000000000003E-2</v>
       </c>
       <c r="M56" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>0.14200000000000002</v>
       </c>
       <c r="N56" s="2">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0.15399999999999991</v>
       </c>
       <c r="O56" s="2">
-        <f t="shared" si="53"/>
+        <f t="shared" si="55"/>
         <v>0.17299999999999993</v>
       </c>
       <c r="P56" s="2">
-        <f t="shared" si="54"/>
+        <f t="shared" si="56"/>
         <v>0.33600000000000002</v>
       </c>
       <c r="R56" s="3" t="s">
@@ -3781,23 +3788,23 @@
         <v>0.12100000000000001</v>
       </c>
       <c r="T56" s="2">
-        <f t="shared" ref="T56" si="66">D56-L$28</f>
+        <f t="shared" ref="T56" si="69">D56-L$28</f>
         <v>-9.5999999999999974E-2</v>
       </c>
       <c r="U56" s="2">
-        <f t="shared" ref="U56" si="67">E56-M$28</f>
+        <f t="shared" ref="U56" si="70">E56-M$28</f>
         <v>0.14599999999999999</v>
       </c>
       <c r="V56" s="2">
-        <f t="shared" ref="V56" si="68">F56-N$28</f>
+        <f t="shared" ref="V56" si="71">F56-N$28</f>
         <v>0.34800000000000003</v>
       </c>
       <c r="W56" s="2">
-        <f t="shared" ref="W56" si="69">G56-O$28</f>
+        <f t="shared" ref="W56" si="72">G56-O$28</f>
         <v>0.37300000000000005</v>
       </c>
       <c r="X56" s="2">
-        <f t="shared" ref="X56" si="70">H56-P$28</f>
+        <f t="shared" ref="X56" si="73">H56-P$28</f>
         <v>0.15100000000000002</v>
       </c>
     </row>
@@ -3827,27 +3834,27 @@
         <v>5</v>
       </c>
       <c r="K57" s="2">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="L57" s="2">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="M57" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="N57" s="2">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="O57" s="2">
-        <f t="shared" si="53"/>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="P57" s="2">
-        <f t="shared" si="54"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="R57" s="3" t="s">
@@ -3858,23 +3865,23 @@
         <v>-2.5000000000000008E-2</v>
       </c>
       <c r="T57" s="2">
-        <f t="shared" ref="T57" si="71">D57-L$29</f>
+        <f t="shared" ref="T57" si="74">D57-L$29</f>
         <v>-0.79499999999999993</v>
       </c>
       <c r="U57" s="2">
-        <f t="shared" ref="U57" si="72">E57-M$29</f>
+        <f t="shared" ref="U57" si="75">E57-M$29</f>
         <v>-8.5000000000000006E-2</v>
       </c>
       <c r="V57" s="2">
-        <f t="shared" ref="V57" si="73">F57-N$29</f>
+        <f t="shared" ref="V57" si="76">F57-N$29</f>
         <v>0.43099999999999994</v>
       </c>
       <c r="W57" s="2">
-        <f t="shared" ref="W57" si="74">G57-O$29</f>
+        <f t="shared" ref="W57" si="77">G57-O$29</f>
         <v>0.53699999999999992</v>
       </c>
       <c r="X57" s="2">
-        <f t="shared" ref="X57" si="75">H57-P$29</f>
+        <f t="shared" ref="X57" si="78">H57-P$29</f>
         <v>-0.109</v>
       </c>
     </row>
@@ -3904,27 +3911,27 @@
         <v>7</v>
       </c>
       <c r="K58" s="2">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>0.65900000000000003</v>
       </c>
       <c r="L58" s="2">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="M58" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>6.2E-2</v>
       </c>
       <c r="N58" s="2">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0.128</v>
       </c>
       <c r="O58" s="2">
-        <f t="shared" si="53"/>
+        <f t="shared" si="55"/>
         <v>0.18700000000000006</v>
       </c>
       <c r="P58" s="2">
-        <f t="shared" si="54"/>
+        <f t="shared" si="56"/>
         <v>0.36099999999999999</v>
       </c>
       <c r="R58" s="3" t="s">
@@ -3935,23 +3942,23 @@
         <v>0.20200000000000001</v>
       </c>
       <c r="T58" s="2">
-        <f t="shared" ref="T58" si="76">D58-L$30</f>
+        <f t="shared" ref="T58" si="79">D58-L$30</f>
         <v>0.27700000000000002</v>
       </c>
       <c r="U58" s="2">
-        <f t="shared" ref="U58" si="77">E58-M$30</f>
+        <f t="shared" ref="U58" si="80">E58-M$30</f>
         <v>0.24100000000000002</v>
       </c>
       <c r="V58" s="2">
-        <f t="shared" ref="V58" si="78">F58-N$30</f>
+        <f t="shared" ref="V58" si="81">F58-N$30</f>
         <v>0.23099999999999998</v>
       </c>
       <c r="W58" s="2">
-        <f t="shared" ref="W58" si="79">G58-O$30</f>
+        <f t="shared" ref="W58" si="82">G58-O$30</f>
         <v>0.16499999999999992</v>
       </c>
       <c r="X58" s="2">
-        <f t="shared" ref="X58" si="80">H58-P$30</f>
+        <f t="shared" ref="X58" si="83">H58-P$30</f>
         <v>0.38300000000000001</v>
       </c>
     </row>
@@ -3981,27 +3988,27 @@
         <v>8</v>
       </c>
       <c r="K59" s="12">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="L59" s="10">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="M59" s="10">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="N59" s="10">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="O59" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="P59" s="10">
-        <f t="shared" si="54"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="R59" s="4" t="s">
@@ -4012,23 +4019,23 @@
         <v>3.7000000000000005E-2</v>
       </c>
       <c r="T59" s="10">
-        <f t="shared" ref="T59" si="81">D59-L$31</f>
+        <f t="shared" ref="T59" si="84">D59-L$31</f>
         <v>0</v>
       </c>
       <c r="U59" s="10">
-        <f t="shared" ref="U59" si="82">E59-M$31</f>
+        <f t="shared" ref="U59" si="85">E59-M$31</f>
         <v>2.2000000000000006E-2</v>
       </c>
       <c r="V59" s="10">
-        <f t="shared" ref="V59" si="83">F59-N$31</f>
+        <f t="shared" ref="V59" si="86">F59-N$31</f>
         <v>0.14499999999999999</v>
       </c>
       <c r="W59" s="10">
-        <f t="shared" ref="W59" si="84">G59-O$31</f>
+        <f t="shared" ref="W59" si="87">G59-O$31</f>
         <v>0.81699999999999995</v>
       </c>
       <c r="X59" s="10">
-        <f t="shared" ref="X59" si="85">H59-P$31</f>
+        <f t="shared" ref="X59" si="88">H59-P$31</f>
         <v>-0.501</v>
       </c>
     </row>
@@ -4037,54 +4044,54 @@
         <v>18</v>
       </c>
       <c r="C60" s="7">
-        <f>SUM(C51:C59)/COUNT(C51:C59)</f>
+        <f t="shared" ref="C60:H60" si="89">SUM(C51:C59)/COUNT(C51:C59)</f>
         <v>0.17055555555555557</v>
       </c>
       <c r="D60" s="7">
-        <f>SUM(D51:D59)/COUNT(D51:D59)</f>
+        <f t="shared" si="89"/>
         <v>0.60599999999999998</v>
       </c>
       <c r="E60" s="7">
-        <f>SUM(E51:E59)/COUNT(E51:E59)</f>
+        <f t="shared" si="89"/>
         <v>0.24388888888888893</v>
       </c>
       <c r="F60" s="7">
-        <f>SUM(F51:F59)/COUNT(F51:F59)</f>
+        <f t="shared" si="89"/>
         <v>0.64822222222222214</v>
       </c>
       <c r="G60" s="7">
-        <f>SUM(G51:G59)/COUNT(G51:G59)</f>
+        <f t="shared" si="89"/>
         <v>0.66355555555555557</v>
       </c>
       <c r="H60" s="7">
-        <f>SUM(H51:H59)/COUNT(H51:H59)</f>
+        <f t="shared" si="89"/>
         <v>0.1331111111111111</v>
       </c>
       <c r="J60" s="3" t="s">
         <v>18</v>
       </c>
       <c r="K60" s="2">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>0.24866666666666665</v>
       </c>
       <c r="L60" s="2">
-        <f t="shared" si="50"/>
+        <f t="shared" si="52"/>
         <v>-4.3444444444444508E-2</v>
       </c>
       <c r="M60" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="53"/>
         <v>9.3777777777777793E-2</v>
       </c>
       <c r="N60" s="2">
-        <f t="shared" si="52"/>
+        <f t="shared" si="54"/>
         <v>0.10044444444444456</v>
       </c>
       <c r="O60" s="2">
-        <f t="shared" si="53"/>
+        <f t="shared" si="55"/>
         <v>0.11755555555555552</v>
       </c>
       <c r="P60" s="2">
-        <f t="shared" si="54"/>
+        <f t="shared" si="56"/>
         <v>0.16244444444444447</v>
       </c>
       <c r="R60" s="3" t="s">
@@ -4095,23 +4102,23 @@
         <v>7.8111111111111131E-2</v>
       </c>
       <c r="T60" s="2">
-        <f t="shared" ref="T60" si="86">D60-L$32</f>
+        <f t="shared" ref="T60" si="90">D60-L$32</f>
         <v>2.011111111111108E-2</v>
       </c>
       <c r="U60" s="2">
-        <f t="shared" ref="U60" si="87">E60-M$32</f>
+        <f t="shared" ref="U60" si="91">E60-M$32</f>
         <v>9.911111111111115E-2</v>
       </c>
       <c r="V60" s="2">
-        <f t="shared" ref="V60" si="88">F60-N$32</f>
+        <f t="shared" ref="V60" si="92">F60-N$32</f>
         <v>0.27622222222222209</v>
       </c>
       <c r="W60" s="2">
-        <f t="shared" ref="W60" si="89">G60-O$32</f>
+        <f t="shared" ref="W60" si="93">G60-O$32</f>
         <v>0.35788888888888892</v>
       </c>
       <c r="X60" s="2">
-        <f t="shared" ref="X60" si="90">H60-P$32</f>
+        <f t="shared" ref="X60" si="94">H60-P$32</f>
         <v>9.1222222222222205E-2</v>
       </c>
     </row>
@@ -4125,77 +4132,77 @@
       </c>
       <c r="D61" s="2">
         <f>(Info!$B$2*Results!D51+Info!$B$3*Results!D52+Info!$B$4*Results!D53+Info!$B$5*Results!D54+Info!$B$6*Results!D55+Info!$B$7*Results!D56+Info!$B$8*Results!D57+Info!$B$9*Results!D58+Info!$B$10*Results!D59)/SUM(Info!$B$2:C$10)</f>
-        <v>0.68913846153846159</v>
+        <v>0.54230024213075056</v>
       </c>
       <c r="E61" s="2">
         <f>(Info!$B$2*Results!E51+Info!$B$3*Results!E52+Info!$B$4*Results!E53+Info!$B$5*Results!E54+Info!$B$6*Results!E55+Info!$B$7*Results!E56+Info!$B$8*Results!E57+Info!$B$9*Results!E58+Info!$B$10*Results!E59)/SUM(Info!$B$2:D$10)</f>
-        <v>0.24690153846153848</v>
+        <v>0.19429297820823246</v>
       </c>
       <c r="F61" s="2">
         <f>(Info!$B$2*Results!F51+Info!$B$3*Results!F52+Info!$B$4*Results!F53+Info!$B$5*Results!F54+Info!$B$6*Results!F55+Info!$B$7*Results!F56+Info!$B$8*Results!F57+Info!$B$9*Results!F58+Info!$B$10*Results!F59)/SUM(Info!$B$2:E$10)</f>
-        <v>0.66288615384615379</v>
+        <v>0.52164164648910405</v>
       </c>
       <c r="G61" s="2">
         <f>(Info!$B$2*Results!G51+Info!$B$3*Results!G52+Info!$B$4*Results!G53+Info!$B$5*Results!G54+Info!$B$6*Results!G55+Info!$B$7*Results!G56+Info!$B$8*Results!G57+Info!$B$9*Results!G58+Info!$B$10*Results!G59)/SUM(Info!$B$2:F$10)</f>
-        <v>0.65804923076923061</v>
+        <v>0.51783535108958823</v>
       </c>
       <c r="H61" s="2">
         <f>(Info!$B$2*Results!H51+Info!$B$3*Results!H52+Info!$B$4*Results!H53+Info!$B$5*Results!H54+Info!$B$6*Results!H55+Info!$B$7*Results!H56+Info!$B$8*Results!H57+Info!$B$9*Results!H58+Info!$B$10*Results!H59)/SUM(Info!$B$2:G$10)</f>
-        <v>0.1666123076923077</v>
+        <v>0.13111138014527846</v>
       </c>
       <c r="J61" s="3" t="s">
         <v>19</v>
       </c>
       <c r="K61" s="2">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>0.22761846153846155</v>
       </c>
       <c r="L61" s="2">
-        <f t="shared" si="50"/>
-        <v>-5.2326153846154022E-2</v>
+        <f t="shared" si="52"/>
+        <v>-4.1176755447941971E-2</v>
       </c>
       <c r="M61" s="2">
-        <f t="shared" si="51"/>
-        <v>8.85723076923077E-2</v>
+        <f t="shared" si="53"/>
+        <v>6.9699757869249396E-2</v>
       </c>
       <c r="N61" s="2">
-        <f t="shared" si="52"/>
-        <v>9.7692307692307745E-2</v>
+        <f t="shared" si="54"/>
+        <v>7.6876513317191364E-2</v>
       </c>
       <c r="O61" s="2">
-        <f t="shared" si="53"/>
-        <v>9.1298461538461662E-2</v>
+        <f t="shared" si="55"/>
+        <v>7.1845036319612698E-2</v>
       </c>
       <c r="P61" s="2">
-        <f t="shared" si="54"/>
-        <v>0.16488615384615382</v>
+        <f t="shared" si="56"/>
+        <v>0.12975302663438254</v>
       </c>
       <c r="R61" s="3" t="s">
         <v>19</v>
       </c>
       <c r="S61" s="2">
         <f>C61-K$33</f>
-        <v>7.789538461538463E-2</v>
+        <v>9.5956937977276974E-2</v>
       </c>
       <c r="T61" s="2">
-        <f t="shared" ref="T61" si="91">D61-L$33</f>
-        <v>5.5273846153846118E-2</v>
+        <f t="shared" ref="T61" si="95">D61-L$33</f>
+        <v>4.3496368038740796E-2</v>
       </c>
       <c r="U61" s="2">
-        <f t="shared" ref="U61" si="92">E61-M$33</f>
-        <v>0.10654769230769232</v>
+        <f t="shared" ref="U61" si="96">E61-M$33</f>
+        <v>8.3845036319612598E-2</v>
       </c>
       <c r="V61" s="2">
-        <f t="shared" ref="V61" si="93">F61-N$33</f>
-        <v>0.28913230769230758</v>
+        <f t="shared" ref="V61" si="97">F61-N$33</f>
+        <v>0.22752542372881346</v>
       </c>
       <c r="W61" s="2">
-        <f t="shared" ref="W61" si="94">G61-O$33</f>
-        <v>0.44034461538461522</v>
+        <f t="shared" ref="W61" si="98">G61-O$33</f>
+        <v>0.34651815980629525</v>
       </c>
       <c r="X61" s="2">
-        <f t="shared" ref="X61" si="95">H61-P$33</f>
-        <v>0.14833538461538462</v>
+        <f t="shared" ref="X61" si="99">H61-P$33</f>
+        <v>0.11672881355932205</v>
       </c>
     </row>
     <row r="63" spans="2:24" x14ac:dyDescent="0.25">
@@ -4208,7 +4215,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B65" s="4" t="s">
         <v>11</v>
       </c>
@@ -4224,17 +4231,29 @@
       <c r="F65" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G65" s="5" t="s">
+      <c r="G65" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H65" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H65" s="5" t="s">
+      <c r="I65" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I65" s="5" t="s">
+      <c r="J65" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K65" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="L65" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="M65" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="66" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="s">
         <v>0</v>
       </c>
@@ -4251,25 +4270,41 @@
       <c r="F66">
         <v>2</v>
       </c>
-      <c r="G66" s="2">
+      <c r="G66">
+        <f>Info!C2-C66</f>
+        <v>8</v>
+      </c>
+      <c r="H66" s="2">
         <f>D66/(D66+E66)</f>
         <v>1</v>
       </c>
-      <c r="H66" s="2">
+      <c r="I66" s="2">
         <f>D66/(D66+F66)</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="I66" s="2">
-        <f>2*G66*H66/(G66+H66)</f>
+      <c r="J66" s="2">
+        <f>2*H66*I66/(H66+I66)</f>
         <v>0.8</v>
       </c>
-    </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K66">
+        <f>(D66+G66)/SUM(D66:G66)</f>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="L66">
+        <f>G66/(G66+E66)</f>
+        <v>1</v>
+      </c>
+      <c r="M66">
+        <f>((D66*G66)-(E66*F66))/SQRT((D66+E66)*(D66+F66)*(G66+E66)*(G66+F66))</f>
+        <v>0.73029674334022143</v>
+      </c>
+    </row>
+    <row r="67" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B67" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C67">
-        <f t="shared" ref="C67:C74" si="96">D67+F67</f>
+        <f t="shared" ref="C67:C74" si="100">D67+F67</f>
         <v>5</v>
       </c>
       <c r="D67">
@@ -4281,25 +4316,41 @@
       <c r="F67">
         <v>0</v>
       </c>
-      <c r="G67" s="2">
-        <f t="shared" ref="G67:G74" si="97">D67/(D67+E67)</f>
-        <v>1</v>
+      <c r="G67">
+        <f>Info!C3-C67</f>
+        <v>6</v>
       </c>
       <c r="H67" s="2">
-        <f t="shared" ref="H67:H74" si="98">D67/(D67+F67)</f>
+        <f>D67/(D67+E67)</f>
         <v>1</v>
       </c>
       <c r="I67" s="2">
-        <f t="shared" ref="I67:I74" si="99">2*G67*H67/(G67+H67)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
+        <f>D67/(D67+F67)</f>
+        <v>1</v>
+      </c>
+      <c r="J67" s="2">
+        <f t="shared" ref="J67:J74" si="101">2*H67*I67/(H67+I67)</f>
+        <v>1</v>
+      </c>
+      <c r="K67">
+        <f t="shared" ref="K67:K74" si="102">(D67+G67)/SUM(D67:G67)</f>
+        <v>1</v>
+      </c>
+      <c r="L67">
+        <f t="shared" ref="L67:L74" si="103">G67/(G67+E67)</f>
+        <v>1</v>
+      </c>
+      <c r="M67">
+        <f t="shared" ref="M67:M74" si="104">((D67*G67)-(E67*F67))/SQRT((D67+E67)*(D67+F67)*(G67+E67)*(G67+F67))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C68">
-        <f t="shared" si="96"/>
+        <f t="shared" si="100"/>
         <v>5</v>
       </c>
       <c r="D68">
@@ -4311,25 +4362,41 @@
       <c r="F68">
         <v>0</v>
       </c>
-      <c r="G68" s="2">
-        <f t="shared" si="97"/>
+      <c r="G68">
+        <f>Info!C4-C68</f>
+        <v>6</v>
+      </c>
+      <c r="H68" s="2">
+        <f>D68/(D68+E68)</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="H68" s="2">
-        <f t="shared" si="98"/>
-        <v>1</v>
-      </c>
       <c r="I68" s="2">
-        <f t="shared" si="99"/>
+        <f>D68/(D68+F68)</f>
+        <v>1</v>
+      </c>
+      <c r="J68" s="2">
+        <f t="shared" si="101"/>
         <v>0.90909090909090906</v>
       </c>
-    </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K68">
+        <f t="shared" si="102"/>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="L68">
+        <f t="shared" si="103"/>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="M68">
+        <f t="shared" si="104"/>
+        <v>0.84515425472851657</v>
+      </c>
+    </row>
+    <row r="69" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B69" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C69">
-        <f t="shared" si="96"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
       <c r="D69">
@@ -4341,16 +4408,20 @@
       <c r="F69">
         <v>0</v>
       </c>
-      <c r="G69" s="2"/>
+      <c r="G69">
+        <f>Info!C5-C69</f>
+        <v>8</v>
+      </c>
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
-    </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J69" s="2"/>
+    </row>
+    <row r="70" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B70" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C70">
-        <f t="shared" si="96"/>
+        <f t="shared" si="100"/>
         <v>1</v>
       </c>
       <c r="D70">
@@ -4362,25 +4433,41 @@
       <c r="F70">
         <v>0</v>
       </c>
-      <c r="G70" s="2">
-        <f t="shared" si="97"/>
-        <v>1</v>
+      <c r="G70">
+        <f>Info!C6-C70</f>
+        <v>7</v>
       </c>
       <c r="H70" s="2">
-        <f t="shared" si="98"/>
+        <f>D70/(D70+E70)</f>
         <v>1</v>
       </c>
       <c r="I70" s="2">
-        <f t="shared" si="99"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
+        <f>D70/(D70+F70)</f>
+        <v>1</v>
+      </c>
+      <c r="J70" s="2">
+        <f t="shared" si="101"/>
+        <v>1</v>
+      </c>
+      <c r="K70">
+        <f t="shared" si="102"/>
+        <v>1</v>
+      </c>
+      <c r="L70">
+        <f t="shared" si="103"/>
+        <v>1</v>
+      </c>
+      <c r="M70">
+        <f t="shared" si="104"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B71" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C71">
-        <f t="shared" si="96"/>
+        <f t="shared" si="100"/>
         <v>1</v>
       </c>
       <c r="D71">
@@ -4392,25 +4479,41 @@
       <c r="F71">
         <v>0</v>
       </c>
-      <c r="G71" s="2">
-        <f t="shared" si="97"/>
-        <v>1</v>
+      <c r="G71">
+        <f>Info!C7-C71</f>
+        <v>11</v>
       </c>
       <c r="H71" s="2">
-        <f t="shared" si="98"/>
+        <f>D71/(D71+E71)</f>
         <v>1</v>
       </c>
       <c r="I71" s="2">
-        <f t="shared" si="99"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
+        <f>D71/(D71+F71)</f>
+        <v>1</v>
+      </c>
+      <c r="J71" s="2">
+        <f t="shared" si="101"/>
+        <v>1</v>
+      </c>
+      <c r="K71">
+        <f t="shared" si="102"/>
+        <v>1</v>
+      </c>
+      <c r="L71">
+        <f t="shared" si="103"/>
+        <v>1</v>
+      </c>
+      <c r="M71">
+        <f t="shared" si="104"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B72" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C72">
-        <f t="shared" si="96"/>
+        <f t="shared" si="100"/>
         <v>6</v>
       </c>
       <c r="D72">
@@ -4422,25 +4525,41 @@
       <c r="F72">
         <v>3</v>
       </c>
-      <c r="G72" s="2">
-        <f t="shared" si="97"/>
+      <c r="G72">
+        <f>Info!C8-C72</f>
+        <v>6</v>
+      </c>
+      <c r="H72" s="2">
+        <f>D72/(D72+E72)</f>
         <v>0.75</v>
       </c>
-      <c r="H72" s="2">
-        <f t="shared" si="98"/>
+      <c r="I72" s="2">
+        <f>D72/(D72+F72)</f>
         <v>0.5</v>
       </c>
-      <c r="I72" s="2">
-        <f t="shared" si="99"/>
+      <c r="J72" s="2">
+        <f t="shared" si="101"/>
         <v>0.6</v>
       </c>
-    </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K72">
+        <f t="shared" si="102"/>
+        <v>0.69230769230769229</v>
+      </c>
+      <c r="L72">
+        <f t="shared" si="103"/>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="M72">
+        <f t="shared" si="104"/>
+        <v>0.38575837490522974</v>
+      </c>
+    </row>
+    <row r="73" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B73" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C73">
-        <f t="shared" si="96"/>
+        <f t="shared" si="100"/>
         <v>1</v>
       </c>
       <c r="D73">
@@ -4452,25 +4571,41 @@
       <c r="F73">
         <v>0</v>
       </c>
-      <c r="G73" s="9">
-        <f t="shared" si="97"/>
-        <v>1</v>
+      <c r="G73">
+        <f>Info!C9-C73</f>
+        <v>5</v>
       </c>
       <c r="H73" s="9">
-        <f t="shared" si="98"/>
+        <f>D73/(D73+E73)</f>
         <v>1</v>
       </c>
       <c r="I73" s="9">
-        <f t="shared" si="99"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
+        <f>D73/(D73+F73)</f>
+        <v>1</v>
+      </c>
+      <c r="J73" s="9">
+        <f t="shared" si="101"/>
+        <v>1</v>
+      </c>
+      <c r="K73">
+        <f t="shared" si="102"/>
+        <v>1</v>
+      </c>
+      <c r="L73">
+        <f t="shared" si="103"/>
+        <v>1</v>
+      </c>
+      <c r="M73">
+        <f t="shared" si="104"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B74" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C74" s="8">
-        <f t="shared" si="96"/>
+        <f t="shared" si="100"/>
         <v>2</v>
       </c>
       <c r="D74" s="5">
@@ -4482,66 +4617,97 @@
       <c r="F74" s="5">
         <v>0</v>
       </c>
-      <c r="G74" s="10">
-        <f t="shared" si="97"/>
+      <c r="G74" s="5">
+        <f>Info!C10-C74</f>
+        <v>4</v>
+      </c>
+      <c r="H74" s="10">
+        <f>D74/(D74+E74)</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="H74" s="10">
-        <f t="shared" si="98"/>
-        <v>1</v>
-      </c>
       <c r="I74" s="10">
-        <f t="shared" si="99"/>
+        <f>D74/(D74+F74)</f>
+        <v>1</v>
+      </c>
+      <c r="J74" s="10">
+        <f t="shared" si="101"/>
         <v>0.8</v>
       </c>
-    </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K74" s="5">
+        <f t="shared" si="102"/>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="L74" s="5">
+        <f t="shared" si="103"/>
+        <v>0.8</v>
+      </c>
+      <c r="M74" s="5">
+        <f t="shared" si="104"/>
+        <v>0.73029674334022143</v>
+      </c>
+    </row>
+    <row r="75" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B75" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D75" s="2">
-        <f>SUM(D66:D74)/COUNT(D66:D74)</f>
-        <v>2.4444444444444446</v>
-      </c>
-      <c r="E75" s="2">
-        <f t="shared" ref="E75:I75" si="100">SUM(E66:E74)/COUNT(E66:E74)</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="F75" s="2">
-        <f t="shared" si="100"/>
-        <v>0.55555555555555558</v>
-      </c>
-      <c r="G75" s="2">
-        <f t="shared" si="100"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+      <c r="H75" s="2">
+        <f>SUM(H66:H74)/COUNT(H66:H74)</f>
         <v>0.90625000000000011</v>
       </c>
-      <c r="H75" s="2">
-        <f t="shared" si="100"/>
+      <c r="I75" s="2">
+        <f>SUM(I66:I74)/COUNT(I66:I74)</f>
         <v>0.89583333333333326</v>
       </c>
-      <c r="I75" s="2">
-        <f t="shared" si="100"/>
+      <c r="J75" s="2">
+        <f>SUM(J66:J74)/COUNT(J66:J74)</f>
         <v>0.88863636363636356</v>
       </c>
-    </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K75" s="2">
+        <f t="shared" ref="K75:M75" si="105">SUM(K66:K74)/COUNT(K66:K74)</f>
+        <v>0.91540750915750912</v>
+      </c>
+      <c r="L75" s="2">
+        <f t="shared" si="105"/>
+        <v>0.93928571428571428</v>
+      </c>
+      <c r="M75" s="2">
+        <f t="shared" si="105"/>
+        <v>0.83643826453927361</v>
+      </c>
+    </row>
+    <row r="76" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B76" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D76" s="11"/>
       <c r="E76" s="11"/>
       <c r="F76" s="11"/>
-      <c r="G76" s="11">
-        <f>(($C66*G66)+($C67*G67)+($C68*G68)+($C69*G69)+($C70*G70)+($C71*G71)+($C72*G72)+($C73*G73)+($C74*G74))/SUM($C66:$C74)</f>
-        <v>0.88888888888888884</v>
-      </c>
       <c r="H76" s="11">
         <f>(($C66*H66)+($C67*H67)+($C68*H68)+($C69*H69)+($C70*H70)+($C71*H71)+($C72*H72)+($C73*H73)+($C74*H74))/SUM($C66:$C74)</f>
-        <v>0.81481481481481477</v>
+        <v>0.88888888888888884</v>
       </c>
       <c r="I76" s="11">
         <f>(($C66*I66)+($C67*I67)+($C68*I68)+($C69*I69)+($C70*I70)+($C71*I71)+($C72*I72)+($C73*I73)+($C74*I74))/SUM($C66:$C74)</f>
+        <v>0.81481481481481477</v>
+      </c>
+      <c r="J76" s="11">
+        <f>(($C66*J66)+($C67*J67)+($C68*J68)+($C69*J69)+($C70*J70)+($C71*J71)+($C72*J72)+($C73*J73)+($C74*J74))/SUM($C66:$C74)</f>
         <v>0.8350168350168351</v>
+      </c>
+      <c r="K76" s="11">
+        <f t="shared" ref="K76:M76" si="106">(($C66*K66)+($C67*K67)+($C68*K68)+($C69*K69)+($C70*K70)+($C71*K71)+($C72*K72)+($C73*K73)+($C74*K74))/SUM($C66:$C74)</f>
+        <v>0.87386379053045715</v>
+      </c>
+      <c r="L76" s="11">
+        <f t="shared" si="106"/>
+        <v>0.92698412698412702</v>
+      </c>
+      <c r="M76" s="11">
+        <f t="shared" si="106"/>
+        <v>0.75491464702947164</v>
       </c>
     </row>
   </sheetData>
@@ -4624,92 +4790,123 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A10"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4">
         <v>60</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6">
         <v>46</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7">
         <v>52</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10">
         <v>9</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Phi/PhiMax to UMM results
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="41">
   <si>
     <t>Mediastore</t>
   </si>
@@ -149,6 +149,12 @@
   <si>
     <t>DELTA Our/SWATTR</t>
   </si>
+  <si>
+    <t>PhiMax</t>
+  </si>
+  <si>
+    <t>Phi/PhiMax</t>
+  </si>
 </sst>
 </file>
 
@@ -254,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -269,6 +275,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -551,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:X89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AC29" sqref="AC29"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="P82" sqref="P82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,7 +569,7 @@
     <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" customWidth="1"/>
     <col min="18" max="18" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -3092,27 +3100,27 @@
         <v>0</v>
       </c>
       <c r="S50" s="2">
-        <f>C64-K$36</f>
+        <f t="shared" ref="S50:X50" si="32">C64-K$36</f>
         <v>1.3000000000000012E-2</v>
       </c>
       <c r="T50" s="2">
-        <f>D64-L$36</f>
+        <f t="shared" si="32"/>
         <v>-6.9000000000000061E-2</v>
       </c>
       <c r="U50" s="2">
-        <f>E64-M$36</f>
+        <f t="shared" si="32"/>
         <v>1.5000000000000013E-2</v>
       </c>
       <c r="V50" s="2">
-        <f>F64-N$36</f>
+        <f t="shared" si="32"/>
         <v>6.5000000000000058E-2</v>
       </c>
       <c r="W50" s="2">
-        <f>G64-O$36</f>
+        <f t="shared" si="32"/>
         <v>7.5000000000000011E-2</v>
       </c>
       <c r="X50" s="2">
-        <f>H64-P$36</f>
+        <f t="shared" si="32"/>
         <v>-2.0000000000000018E-3</v>
       </c>
     </row>
@@ -3142,54 +3150,54 @@
         <v>1</v>
       </c>
       <c r="K51" s="2">
-        <f t="shared" ref="K51:K57" si="32">C37-C51</f>
+        <f t="shared" ref="K51:K57" si="33">C37-C51</f>
         <v>0.64900000000000002</v>
       </c>
       <c r="L51" s="2">
-        <f t="shared" ref="L51:L58" si="33">D37-D51</f>
+        <f t="shared" ref="L51:L58" si="34">D37-D51</f>
         <v>-3.7000000000000033E-2</v>
       </c>
       <c r="M51" s="2">
-        <f t="shared" ref="M51:M58" si="34">E37-E51</f>
+        <f t="shared" ref="M51:M58" si="35">E37-E51</f>
         <v>0.35000000000000003</v>
       </c>
       <c r="N51" s="2">
-        <f t="shared" ref="N51:N58" si="35">F37-F51</f>
+        <f t="shared" ref="N51:N58" si="36">F37-F51</f>
         <v>0.16299999999999992</v>
       </c>
       <c r="O51" s="2">
-        <f t="shared" ref="O51:O58" si="36">G37-G51</f>
+        <f t="shared" ref="O51:O58" si="37">G37-G51</f>
         <v>0.18899999999999995</v>
       </c>
       <c r="P51" s="2">
-        <f t="shared" ref="P51:P58" si="37">H37-H51</f>
+        <f t="shared" ref="P51:P58" si="38">H37-H51</f>
         <v>0.5</v>
       </c>
       <c r="R51" s="3" t="s">
         <v>1</v>
       </c>
       <c r="S51" s="2">
-        <f>C65-K$37</f>
+        <f t="shared" ref="S51:X51" si="39">C65-K$37</f>
         <v>0.11</v>
       </c>
       <c r="T51" s="2">
-        <f>D65-L$37</f>
+        <f t="shared" si="39"/>
         <v>3.7000000000000033E-2</v>
       </c>
       <c r="U51" s="2">
-        <f>E65-M$37</f>
+        <f t="shared" si="39"/>
         <v>0.14300000000000002</v>
       </c>
       <c r="V51" s="2">
-        <f>F65-N$37</f>
+        <f t="shared" si="39"/>
         <v>0.31200000000000006</v>
       </c>
       <c r="W51" s="2">
-        <f>G65-O$37</f>
+        <f t="shared" si="39"/>
         <v>0.35100000000000003</v>
       </c>
       <c r="X51" s="2">
-        <f>H65-P$37</f>
+        <f t="shared" si="39"/>
         <v>0.17799999999999999</v>
       </c>
     </row>
@@ -3219,54 +3227,54 @@
         <v>6</v>
       </c>
       <c r="K52" s="2">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="L52" s="2">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="M52" s="2">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="N52" s="2">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="O52" s="2">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="P52" s="2">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="R52" s="3" t="s">
         <v>6</v>
       </c>
       <c r="S52" s="2">
-        <f>C52-K$38</f>
+        <f t="shared" ref="S52:X52" si="40">C52-K$38</f>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="T52" s="2">
-        <f>D52-L$38</f>
+        <f t="shared" si="40"/>
         <v>0.5</v>
       </c>
       <c r="U52" s="2">
-        <f>E52-M$38</f>
+        <f t="shared" si="40"/>
         <v>0.12300000000000003</v>
       </c>
       <c r="V52" s="2">
-        <f>F52-N$38</f>
+        <f t="shared" si="40"/>
         <v>-9.000000000000008E-3</v>
       </c>
       <c r="W52" s="2">
-        <f>G52-O$38</f>
+        <f t="shared" si="40"/>
         <v>-8.3000000000000018E-2</v>
       </c>
       <c r="X52" s="2">
-        <f>H52-P$38</f>
+        <f t="shared" si="40"/>
         <v>0.19600000000000001</v>
       </c>
     </row>
@@ -3296,54 +3304,54 @@
         <v>2</v>
       </c>
       <c r="K53" s="2">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>6.699999999999999E-2</v>
       </c>
       <c r="L53" s="2">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>-2.0000000000000018E-2</v>
       </c>
       <c r="M53" s="2">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>9.099999999999997E-2</v>
       </c>
       <c r="N53" s="2">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.11699999999999999</v>
       </c>
       <c r="O53" s="2">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0.122</v>
       </c>
       <c r="P53" s="2">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>9.099999999999997E-2</v>
       </c>
       <c r="R53" s="3" t="s">
         <v>2</v>
       </c>
       <c r="S53" s="2">
-        <f>C53-K$39</f>
+        <f t="shared" ref="S53:X53" si="41">C53-K$39</f>
         <v>7.8E-2</v>
       </c>
       <c r="T53" s="2">
-        <f>D53-L$39</f>
+        <f t="shared" si="41"/>
         <v>0.18000000000000005</v>
       </c>
       <c r="U53" s="2">
-        <f>E53-M$39</f>
+        <f t="shared" si="41"/>
         <v>0.129</v>
       </c>
       <c r="V53" s="2">
-        <f>F53-N$39</f>
+        <f t="shared" si="41"/>
         <v>0.435</v>
       </c>
       <c r="W53" s="2">
-        <f>G53-O$39</f>
+        <f t="shared" si="41"/>
         <v>0.443</v>
       </c>
       <c r="X53" s="2">
-        <f>H53-P$39</f>
+        <f t="shared" si="41"/>
         <v>0.24100000000000002</v>
       </c>
     </row>
@@ -3373,54 +3381,54 @@
         <v>3</v>
       </c>
       <c r="K54" s="2">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.8000000000000025E-2</v>
       </c>
       <c r="L54" s="2">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>-2.200000000000002E-2</v>
       </c>
       <c r="M54" s="2">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="N54" s="2">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>3.7000000000000033E-2</v>
       </c>
       <c r="O54" s="2">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>3.9000000000000035E-2</v>
       </c>
       <c r="P54" s="2">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="R54" s="3" t="s">
         <v>3</v>
       </c>
       <c r="S54" s="2">
-        <f>C54-K$40</f>
+        <f t="shared" ref="S54:X54" si="42">C54-K$40</f>
         <v>0.10599999999999998</v>
       </c>
       <c r="T54" s="2">
-        <f>D54-L$40</f>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="U54" s="2">
-        <f>E54-M$40</f>
+        <f t="shared" si="42"/>
         <v>0.16600000000000001</v>
       </c>
       <c r="V54" s="2">
-        <f>F54-N$40</f>
+        <f t="shared" si="42"/>
         <v>0.57599999999999996</v>
       </c>
       <c r="W54" s="2">
-        <f>G54-O$40</f>
+        <f t="shared" si="42"/>
         <v>0.59799999999999998</v>
       </c>
       <c r="X54" s="2">
-        <f>H54-P$40</f>
+        <f t="shared" si="42"/>
         <v>0.26700000000000002</v>
       </c>
     </row>
@@ -3450,54 +3458,54 @@
         <v>4</v>
       </c>
       <c r="K55" s="2">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.63100000000000001</v>
       </c>
       <c r="L55" s="2">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>-9.600000000000003E-2</v>
       </c>
       <c r="M55" s="2">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>9.099999999999997E-2</v>
       </c>
       <c r="N55" s="2">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>9.8999999999999977E-2</v>
       </c>
       <c r="O55" s="2">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0.11299999999999999</v>
       </c>
       <c r="P55" s="2">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0.27300000000000002</v>
       </c>
       <c r="R55" s="3" t="s">
         <v>4</v>
       </c>
       <c r="S55" s="2">
-        <f>C55-K$41</f>
+        <f t="shared" ref="S55:X55" si="43">C55-K$41</f>
         <v>0.17499999999999999</v>
       </c>
       <c r="T55" s="2">
-        <f>D55-L$41</f>
+        <f t="shared" si="43"/>
         <v>-9.5999999999999974E-2</v>
       </c>
       <c r="U55" s="2">
-        <f>E55-M$41</f>
+        <f t="shared" si="43"/>
         <v>0.19700000000000004</v>
       </c>
       <c r="V55" s="2">
-        <f>F55-N$41</f>
+        <f t="shared" si="43"/>
         <v>0.40299999999999997</v>
       </c>
       <c r="W55" s="2">
-        <f>G55-O$41</f>
+        <f t="shared" si="43"/>
         <v>0.433</v>
       </c>
       <c r="X55" s="2">
-        <f>H55-P$41</f>
+        <f t="shared" si="43"/>
         <v>0.21400000000000002</v>
       </c>
     </row>
@@ -3527,54 +3535,54 @@
         <v>5</v>
       </c>
       <c r="K56" s="2">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="L56" s="2">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="M56" s="2">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="N56" s="2">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="O56" s="2">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="P56" s="2">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="R56" s="3" t="s">
         <v>5</v>
       </c>
       <c r="S56" s="2">
-        <f>C56-K$42</f>
+        <f t="shared" ref="S56:X56" si="44">C56-K$42</f>
         <v>-2.5000000000000008E-2</v>
       </c>
       <c r="T56" s="2">
-        <f>D56-L$42</f>
+        <f t="shared" si="44"/>
         <v>-0.79499999999999993</v>
       </c>
       <c r="U56" s="2">
-        <f>E56-M$42</f>
+        <f t="shared" si="44"/>
         <v>-8.5000000000000006E-2</v>
       </c>
       <c r="V56" s="2">
-        <f>F56-N$42</f>
+        <f t="shared" si="44"/>
         <v>0.43099999999999994</v>
       </c>
       <c r="W56" s="2">
-        <f>G56-O$42</f>
+        <f t="shared" si="44"/>
         <v>0.53699999999999992</v>
       </c>
       <c r="X56" s="2">
-        <f>H56-P$42</f>
+        <f t="shared" si="44"/>
         <v>-0.109</v>
       </c>
     </row>
@@ -3604,54 +3612,54 @@
         <v>7</v>
       </c>
       <c r="K57" s="2">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="L57" s="2">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="M57" s="2">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="N57" s="2">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="O57" s="2">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="P57" s="2">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="R57" s="3" t="s">
         <v>7</v>
       </c>
       <c r="S57" s="2">
-        <f>C57-K$43</f>
+        <f t="shared" ref="S57:X57" si="45">C57-K$43</f>
         <v>0.86099999999999999</v>
       </c>
       <c r="T57" s="2">
-        <f>D57-L$43</f>
+        <f t="shared" si="45"/>
         <v>0.27700000000000002</v>
       </c>
       <c r="U57" s="2">
-        <f>E57-M$43</f>
+        <f t="shared" si="45"/>
         <v>0.30300000000000005</v>
       </c>
       <c r="V57" s="2">
-        <f>F57-N$43</f>
+        <f t="shared" si="45"/>
         <v>0.35899999999999999</v>
       </c>
       <c r="W57" s="2">
-        <f>G57-O$43</f>
+        <f t="shared" si="45"/>
         <v>0.35199999999999998</v>
       </c>
       <c r="X57" s="2">
-        <f>H57-P$43</f>
+        <f t="shared" si="45"/>
         <v>0.74399999999999999</v>
       </c>
     </row>
@@ -3685,50 +3693,50 @@
         <v>0</v>
       </c>
       <c r="L58" s="10">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="M58" s="10">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="N58" s="10">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="O58" s="10">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="P58" s="10">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="R58" s="4" t="s">
         <v>8</v>
       </c>
       <c r="S58" s="12">
-        <f>C58-K$44</f>
+        <f t="shared" ref="S58:X58" si="46">C58-K$44</f>
         <v>3.7000000000000005E-2</v>
       </c>
       <c r="T58" s="10">
-        <f>D58-L$44</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="U58" s="10">
-        <f>E58-M$44</f>
+        <f t="shared" si="46"/>
         <v>2.2000000000000006E-2</v>
       </c>
       <c r="V58" s="10">
-        <f>F58-N$44</f>
+        <f t="shared" si="46"/>
         <v>0.14499999999999999</v>
       </c>
       <c r="W58" s="10">
-        <f>G58-O$44</f>
+        <f t="shared" si="46"/>
         <v>0.81699999999999995</v>
       </c>
       <c r="X58" s="10">
-        <f>H58-P$44</f>
+        <f t="shared" si="46"/>
         <v>-0.501</v>
       </c>
     </row>
@@ -3741,15 +3749,15 @@
         <v>0.26044444444444448</v>
       </c>
       <c r="D59" s="7">
-        <f t="shared" ref="D59:F59" si="38">SUM(D50:D58)/COUNT(D50:D58)</f>
+        <f t="shared" ref="D59:F59" si="47">SUM(D50:D58)/COUNT(D50:D58)</f>
         <v>0.58966666666666656</v>
       </c>
       <c r="E59" s="7">
-        <f t="shared" si="38"/>
+        <f t="shared" si="47"/>
         <v>0.26766666666666672</v>
       </c>
       <c r="F59" s="7">
-        <f t="shared" si="38"/>
+        <f t="shared" si="47"/>
         <v>0.68655555555555559</v>
       </c>
       <c r="G59" s="7">
@@ -3757,61 +3765,61 @@
         <v>0.71144444444444455</v>
       </c>
       <c r="H59" s="7">
-        <f t="shared" ref="H59" si="39">SUM(H50:H58)/COUNT(H50:H58)</f>
+        <f t="shared" ref="H59" si="48">SUM(H50:H58)/COUNT(H50:H58)</f>
         <v>0.19011111111111109</v>
       </c>
       <c r="J59" s="3" t="s">
         <v>18</v>
       </c>
       <c r="K59" s="2">
-        <f t="shared" ref="K59:K60" si="40">C45-C59</f>
+        <f t="shared" ref="K59:K60" si="49">C45-C59</f>
         <v>0.15877777777777774</v>
       </c>
       <c r="L59" s="2">
-        <f t="shared" ref="L59:L60" si="41">D45-D59</f>
+        <f t="shared" ref="L59:L60" si="50">D45-D59</f>
         <v>-2.7111111111111086E-2</v>
       </c>
       <c r="M59" s="2">
-        <f t="shared" ref="M59:M60" si="42">E45-E59</f>
+        <f t="shared" ref="M59:M60" si="51">E45-E59</f>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="N59" s="2">
-        <f t="shared" ref="N59:N60" si="43">F45-F59</f>
+        <f t="shared" ref="N59:N60" si="52">F45-F59</f>
         <v>6.2111111111111117E-2</v>
       </c>
       <c r="O59" s="2">
-        <f t="shared" ref="O59:O60" si="44">G45-G59</f>
+        <f t="shared" ref="O59:O60" si="53">G45-G59</f>
         <v>6.9666666666666544E-2</v>
       </c>
       <c r="P59" s="2">
-        <f t="shared" ref="P59:P60" si="45">H45-H59</f>
+        <f t="shared" ref="P59:P60" si="54">H45-H59</f>
         <v>0.10544444444444448</v>
       </c>
       <c r="R59" s="3" t="s">
         <v>18</v>
       </c>
       <c r="S59" s="2">
-        <f>C59-K$45</f>
+        <f t="shared" ref="S59:X59" si="55">C59-K$45</f>
         <v>0.16800000000000004</v>
       </c>
       <c r="T59" s="2">
-        <f>D59-L$45</f>
+        <f t="shared" si="55"/>
         <v>3.7777777777776578E-3</v>
       </c>
       <c r="U59" s="2">
-        <f>E59-M$45</f>
+        <f t="shared" si="55"/>
         <v>0.12288888888888894</v>
       </c>
       <c r="V59" s="2">
-        <f>F59-N$45</f>
+        <f t="shared" si="55"/>
         <v>0.31455555555555553</v>
       </c>
       <c r="W59" s="2">
-        <f>G59-O$45</f>
+        <f t="shared" si="55"/>
         <v>0.4057777777777779</v>
       </c>
       <c r="X59" s="2">
-        <f>H59-P$45</f>
+        <f t="shared" si="55"/>
         <v>0.1482222222222222</v>
       </c>
     </row>
@@ -3847,54 +3855,54 @@
         <v>19</v>
       </c>
       <c r="K60" s="2">
-        <f t="shared" si="40"/>
+        <f t="shared" si="49"/>
         <v>0.18119384615384615</v>
       </c>
       <c r="L60" s="2">
-        <f t="shared" si="41"/>
+        <f t="shared" si="50"/>
         <v>-2.4222760290557033E-2</v>
       </c>
       <c r="M60" s="2">
-        <f t="shared" si="42"/>
+        <f t="shared" si="51"/>
         <v>5.9675544794188851E-2</v>
       </c>
       <c r="N60" s="2">
-        <f t="shared" si="43"/>
+        <f t="shared" si="52"/>
         <v>5.8900726392251856E-2</v>
       </c>
       <c r="O60" s="2">
-        <f t="shared" si="44"/>
+        <f t="shared" si="53"/>
         <v>6.5646489104116301E-2</v>
       </c>
       <c r="P60" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="54"/>
         <v>9.2338983050847395E-2</v>
       </c>
       <c r="R60" s="3" t="s">
         <v>19</v>
       </c>
       <c r="S60" s="2">
-        <f>C60-K$46</f>
+        <f t="shared" ref="S60:X60" si="56">C60-K$46</f>
         <v>0.14238155336189237</v>
       </c>
       <c r="T60" s="2">
-        <f>D60-L$46</f>
+        <f t="shared" si="56"/>
         <v>2.6542372881355858E-2</v>
       </c>
       <c r="U60" s="2">
-        <f>E60-M$46</f>
+        <f t="shared" si="56"/>
         <v>9.3869249394673143E-2</v>
       </c>
       <c r="V60" s="2">
-        <f>F60-N$46</f>
+        <f t="shared" si="56"/>
         <v>0.24550121065375297</v>
       </c>
       <c r="W60" s="2">
-        <f>G60-O$46</f>
+        <f t="shared" si="56"/>
         <v>0.35271670702179164</v>
       </c>
       <c r="X60" s="2">
-        <f>H60-P$46</f>
+        <f t="shared" si="56"/>
         <v>0.15414285714285719</v>
       </c>
     </row>
@@ -4007,50 +4015,50 @@
         <v>5.3999999999999992E-2</v>
       </c>
       <c r="L64" s="2">
-        <f t="shared" ref="L64:P64" si="46">D36-D64</f>
+        <f t="shared" ref="L64:P64" si="57">D36-D64</f>
         <v>-6.899999999999995E-2</v>
       </c>
       <c r="M64" s="2">
-        <f t="shared" si="46"/>
+        <f t="shared" si="57"/>
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="N64" s="2">
-        <f t="shared" si="46"/>
+        <f t="shared" si="57"/>
         <v>0.1429999999999999</v>
       </c>
       <c r="O64" s="2">
-        <f t="shared" si="46"/>
+        <f t="shared" si="57"/>
         <v>0.16399999999999992</v>
       </c>
       <c r="P64" s="2">
-        <f t="shared" si="46"/>
+        <f t="shared" si="57"/>
         <v>5.3000000000000019E-2</v>
       </c>
       <c r="R64" s="3" t="s">
         <v>0</v>
       </c>
       <c r="S64" s="2">
-        <f>C64-K$36</f>
+        <f t="shared" ref="S64:X64" si="58">C64-K$36</f>
         <v>1.3000000000000012E-2</v>
       </c>
       <c r="T64" s="2">
-        <f>D64-L$36</f>
+        <f t="shared" si="58"/>
         <v>-6.9000000000000061E-2</v>
       </c>
       <c r="U64" s="2">
-        <f>E64-M$36</f>
+        <f t="shared" si="58"/>
         <v>1.5000000000000013E-2</v>
       </c>
       <c r="V64" s="2">
-        <f>F64-N$36</f>
+        <f t="shared" si="58"/>
         <v>6.5000000000000058E-2</v>
       </c>
       <c r="W64" s="2">
-        <f>G64-O$36</f>
+        <f t="shared" si="58"/>
         <v>7.5000000000000011E-2</v>
       </c>
       <c r="X64" s="2">
-        <f>H64-P$36</f>
+        <f t="shared" si="58"/>
         <v>-2.0000000000000018E-3</v>
       </c>
     </row>
@@ -4080,54 +4088,54 @@
         <v>1</v>
       </c>
       <c r="K65" s="2">
-        <f t="shared" ref="K65:K74" si="47">C37-C65</f>
+        <f t="shared" ref="K65:K74" si="59">C37-C65</f>
         <v>0.73599999999999999</v>
       </c>
       <c r="L65" s="2">
-        <f t="shared" ref="L65:L74" si="48">D37-D65</f>
+        <f t="shared" ref="L65:L74" si="60">D37-D65</f>
         <v>-3.7000000000000033E-2</v>
       </c>
       <c r="M65" s="2">
-        <f t="shared" ref="M65:M74" si="49">E37-E65</f>
+        <f t="shared" ref="M65:M74" si="61">E37-E65</f>
         <v>0.443</v>
       </c>
       <c r="N65" s="2">
-        <f t="shared" ref="N65:N74" si="50">F37-F65</f>
+        <f t="shared" ref="N65:N74" si="62">F37-F65</f>
         <v>0.27699999999999991</v>
       </c>
       <c r="O65" s="2">
-        <f t="shared" ref="O65:O74" si="51">G37-G65</f>
+        <f t="shared" ref="O65:O74" si="63">G37-G65</f>
         <v>0.31799999999999995</v>
       </c>
       <c r="P65" s="2">
-        <f t="shared" ref="P65:P74" si="52">H37-H65</f>
+        <f t="shared" ref="P65:P74" si="64">H37-H65</f>
         <v>0.60500000000000009</v>
       </c>
       <c r="R65" s="3" t="s">
         <v>1</v>
       </c>
       <c r="S65" s="2">
-        <f>C65-K$37</f>
+        <f t="shared" ref="S65:X65" si="65">C65-K$37</f>
         <v>0.11</v>
       </c>
       <c r="T65" s="2">
-        <f>D65-L$37</f>
+        <f t="shared" si="65"/>
         <v>3.7000000000000033E-2</v>
       </c>
       <c r="U65" s="2">
-        <f>E65-M$37</f>
+        <f t="shared" si="65"/>
         <v>0.14300000000000002</v>
       </c>
       <c r="V65" s="2">
-        <f>F65-N$37</f>
+        <f t="shared" si="65"/>
         <v>0.31200000000000006</v>
       </c>
       <c r="W65" s="2">
-        <f>G65-O$37</f>
+        <f t="shared" si="65"/>
         <v>0.35100000000000003</v>
       </c>
       <c r="X65" s="2">
-        <f>H65-P$37</f>
+        <f t="shared" si="65"/>
         <v>0.17799999999999999</v>
       </c>
     </row>
@@ -4157,54 +4165,54 @@
         <v>6</v>
       </c>
       <c r="K66" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="59"/>
         <v>0</v>
       </c>
       <c r="L66" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="M66" s="2">
-        <f t="shared" si="49"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="N66" s="2">
-        <f t="shared" si="50"/>
+        <f t="shared" si="62"/>
         <v>0</v>
       </c>
       <c r="O66" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="P66" s="2">
-        <f t="shared" si="52"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="R66" s="3" t="s">
         <v>6</v>
       </c>
       <c r="S66" s="2">
-        <f>C66-K$38</f>
+        <f t="shared" ref="S66:X66" si="66">C66-K$38</f>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="T66" s="2">
-        <f>D66-L$38</f>
+        <f t="shared" si="66"/>
         <v>0.5</v>
       </c>
       <c r="U66" s="2">
-        <f>E66-M$38</f>
+        <f t="shared" si="66"/>
         <v>0.12300000000000003</v>
       </c>
       <c r="V66" s="2">
-        <f>F66-N$38</f>
+        <f t="shared" si="66"/>
         <v>-9.000000000000008E-3</v>
       </c>
       <c r="W66" s="2">
-        <f>G66-O$38</f>
+        <f t="shared" si="66"/>
         <v>-8.3000000000000018E-2</v>
       </c>
       <c r="X66" s="2">
-        <f>H66-P$38</f>
+        <f t="shared" si="66"/>
         <v>0.19600000000000001</v>
       </c>
     </row>
@@ -4234,54 +4242,54 @@
         <v>2</v>
       </c>
       <c r="K67" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="59"/>
         <v>6.7999999999999991E-2</v>
       </c>
       <c r="L67" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="60"/>
         <v>-7.999999999999996E-2</v>
       </c>
       <c r="M67" s="2">
-        <f t="shared" si="49"/>
+        <f t="shared" si="61"/>
         <v>9.1999999999999971E-2</v>
       </c>
       <c r="N67" s="2">
-        <f t="shared" si="50"/>
+        <f t="shared" si="62"/>
         <v>0.13</v>
       </c>
       <c r="O67" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="63"/>
         <v>0.13700000000000001</v>
       </c>
       <c r="P67" s="2">
-        <f t="shared" si="52"/>
+        <f t="shared" si="64"/>
         <v>7.6999999999999985E-2</v>
       </c>
       <c r="R67" s="3" t="s">
         <v>2</v>
       </c>
       <c r="S67" s="2">
-        <f>C67-K$39</f>
+        <f t="shared" ref="S67:X67" si="67">C67-K$39</f>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="T67" s="2">
-        <f>D67-L$39</f>
+        <f t="shared" si="67"/>
         <v>0.24</v>
       </c>
       <c r="U67" s="2">
-        <f>E67-M$39</f>
+        <f t="shared" si="67"/>
         <v>0.128</v>
       </c>
       <c r="V67" s="2">
-        <f>F67-N$39</f>
+        <f t="shared" si="67"/>
         <v>0.42199999999999999</v>
       </c>
       <c r="W67" s="2">
-        <f>G67-O$39</f>
+        <f t="shared" si="67"/>
         <v>0.42799999999999999</v>
       </c>
       <c r="X67" s="2">
-        <f>H67-P$39</f>
+        <f t="shared" si="67"/>
         <v>0.255</v>
       </c>
     </row>
@@ -4311,54 +4319,54 @@
         <v>3</v>
       </c>
       <c r="K68" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="59"/>
         <v>3.6000000000000004E-2</v>
       </c>
       <c r="L68" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="60"/>
         <v>-0.10899999999999999</v>
       </c>
       <c r="M68" s="2">
-        <f t="shared" si="49"/>
+        <f t="shared" si="61"/>
         <v>4.0000000000000008E-2</v>
       </c>
       <c r="N68" s="2">
-        <f t="shared" si="50"/>
+        <f t="shared" si="62"/>
         <v>7.1999999999999953E-2</v>
       </c>
       <c r="O68" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="63"/>
         <v>7.8999999999999959E-2</v>
       </c>
       <c r="P68" s="2">
-        <f t="shared" si="52"/>
+        <f t="shared" si="64"/>
         <v>0.03</v>
       </c>
       <c r="R68" s="3" t="s">
         <v>3</v>
       </c>
       <c r="S68" s="2">
-        <f>C68-K$40</f>
+        <f t="shared" ref="S68:X68" si="68">C68-K$40</f>
         <v>9.8000000000000004E-2</v>
       </c>
       <c r="T68" s="2">
-        <f>D68-L$40</f>
+        <f t="shared" si="68"/>
         <v>8.6999999999999966E-2</v>
       </c>
       <c r="U68" s="2">
-        <f>E68-M$40</f>
+        <f t="shared" si="68"/>
         <v>0.159</v>
       </c>
       <c r="V68" s="2">
-        <f>F68-N$40</f>
+        <f t="shared" si="68"/>
         <v>0.54100000000000004</v>
       </c>
       <c r="W68" s="2">
-        <f>G68-O$40</f>
+        <f t="shared" si="68"/>
         <v>0.55800000000000005</v>
       </c>
       <c r="X68" s="2">
-        <f>H68-P$40</f>
+        <f t="shared" si="68"/>
         <v>0.27</v>
       </c>
     </row>
@@ -4388,54 +4396,54 @@
         <v>4</v>
       </c>
       <c r="K69" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="59"/>
         <v>0.68500000000000005</v>
       </c>
       <c r="L69" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="60"/>
         <v>-9.600000000000003E-2</v>
       </c>
       <c r="M69" s="2">
-        <f t="shared" si="49"/>
+        <f t="shared" si="61"/>
         <v>0.14200000000000002</v>
       </c>
       <c r="N69" s="2">
-        <f t="shared" si="50"/>
+        <f t="shared" si="62"/>
         <v>0.15399999999999991</v>
       </c>
       <c r="O69" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="63"/>
         <v>0.17299999999999993</v>
       </c>
       <c r="P69" s="2">
-        <f t="shared" si="52"/>
+        <f t="shared" si="64"/>
         <v>0.33600000000000002</v>
       </c>
       <c r="R69" s="3" t="s">
         <v>4</v>
       </c>
       <c r="S69" s="2">
-        <f>C69-K$41</f>
+        <f t="shared" ref="S69:X69" si="69">C69-K$41</f>
         <v>0.12100000000000001</v>
       </c>
       <c r="T69" s="2">
-        <f>D69-L$41</f>
+        <f t="shared" si="69"/>
         <v>-9.5999999999999974E-2</v>
       </c>
       <c r="U69" s="2">
-        <f>E69-M$41</f>
+        <f t="shared" si="69"/>
         <v>0.14599999999999999</v>
       </c>
       <c r="V69" s="2">
-        <f>F69-N$41</f>
+        <f t="shared" si="69"/>
         <v>0.34800000000000003</v>
       </c>
       <c r="W69" s="2">
-        <f>G69-O$41</f>
+        <f t="shared" si="69"/>
         <v>0.37300000000000005</v>
       </c>
       <c r="X69" s="2">
-        <f>H69-P$41</f>
+        <f t="shared" si="69"/>
         <v>0.15100000000000002</v>
       </c>
     </row>
@@ -4465,54 +4473,54 @@
         <v>5</v>
       </c>
       <c r="K70" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="59"/>
         <v>0</v>
       </c>
       <c r="L70" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="M70" s="2">
-        <f t="shared" si="49"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="N70" s="2">
-        <f t="shared" si="50"/>
+        <f t="shared" si="62"/>
         <v>0</v>
       </c>
       <c r="O70" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="P70" s="2">
-        <f t="shared" si="52"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="R70" s="3" t="s">
         <v>5</v>
       </c>
       <c r="S70" s="2">
-        <f>C70-K$42</f>
+        <f t="shared" ref="S70:X70" si="70">C70-K$42</f>
         <v>-2.5000000000000008E-2</v>
       </c>
       <c r="T70" s="2">
-        <f>D70-L$42</f>
+        <f t="shared" si="70"/>
         <v>-0.79499999999999993</v>
       </c>
       <c r="U70" s="2">
-        <f>E70-M$42</f>
+        <f t="shared" si="70"/>
         <v>-8.5000000000000006E-2</v>
       </c>
       <c r="V70" s="2">
-        <f>F70-N$42</f>
+        <f t="shared" si="70"/>
         <v>0.43099999999999994</v>
       </c>
       <c r="W70" s="2">
-        <f>G70-O$42</f>
+        <f t="shared" si="70"/>
         <v>0.53699999999999992</v>
       </c>
       <c r="X70" s="2">
-        <f>H70-P$42</f>
+        <f t="shared" si="70"/>
         <v>-0.109</v>
       </c>
     </row>
@@ -4542,54 +4550,54 @@
         <v>7</v>
       </c>
       <c r="K71" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="59"/>
         <v>0.65900000000000003</v>
       </c>
       <c r="L71" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="M71" s="2">
-        <f t="shared" si="49"/>
+        <f t="shared" si="61"/>
         <v>6.2E-2</v>
       </c>
       <c r="N71" s="2">
-        <f t="shared" si="50"/>
+        <f t="shared" si="62"/>
         <v>0.128</v>
       </c>
       <c r="O71" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="63"/>
         <v>0.18700000000000006</v>
       </c>
       <c r="P71" s="2">
-        <f t="shared" si="52"/>
+        <f t="shared" si="64"/>
         <v>0.36099999999999999</v>
       </c>
       <c r="R71" s="3" t="s">
         <v>7</v>
       </c>
       <c r="S71" s="2">
-        <f>C71-K$43</f>
+        <f t="shared" ref="S71:X71" si="71">C71-K$43</f>
         <v>0.20200000000000001</v>
       </c>
       <c r="T71" s="2">
-        <f>D71-L$43</f>
+        <f t="shared" si="71"/>
         <v>0.27700000000000002</v>
       </c>
       <c r="U71" s="2">
-        <f>E71-M$43</f>
+        <f t="shared" si="71"/>
         <v>0.24100000000000002</v>
       </c>
       <c r="V71" s="2">
-        <f>F71-N$43</f>
+        <f t="shared" si="71"/>
         <v>0.23099999999999998</v>
       </c>
       <c r="W71" s="2">
-        <f>G71-O$43</f>
+        <f t="shared" si="71"/>
         <v>0.16499999999999992</v>
       </c>
       <c r="X71" s="2">
-        <f>H71-P$43</f>
+        <f t="shared" si="71"/>
         <v>0.38300000000000001</v>
       </c>
     </row>
@@ -4619,54 +4627,54 @@
         <v>8</v>
       </c>
       <c r="K72" s="12">
-        <f t="shared" si="47"/>
+        <f t="shared" si="59"/>
         <v>0</v>
       </c>
       <c r="L72" s="10">
-        <f t="shared" si="48"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="M72" s="10">
-        <f t="shared" si="49"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="N72" s="10">
-        <f t="shared" si="50"/>
+        <f t="shared" si="62"/>
         <v>0</v>
       </c>
       <c r="O72" s="10">
-        <f t="shared" si="51"/>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="P72" s="10">
-        <f t="shared" si="52"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="R72" s="4" t="s">
         <v>8</v>
       </c>
       <c r="S72" s="12">
-        <f>C72-K$44</f>
+        <f t="shared" ref="S72:X72" si="72">C72-K$44</f>
         <v>3.7000000000000005E-2</v>
       </c>
       <c r="T72" s="10">
-        <f>D72-L$44</f>
+        <f t="shared" si="72"/>
         <v>0</v>
       </c>
       <c r="U72" s="10">
-        <f>E72-M$44</f>
+        <f t="shared" si="72"/>
         <v>2.2000000000000006E-2</v>
       </c>
       <c r="V72" s="10">
-        <f>F72-N$44</f>
+        <f t="shared" si="72"/>
         <v>0.14499999999999999</v>
       </c>
       <c r="W72" s="10">
-        <f>G72-O$44</f>
+        <f t="shared" si="72"/>
         <v>0.81699999999999995</v>
       </c>
       <c r="X72" s="10">
-        <f>H72-P$44</f>
+        <f t="shared" si="72"/>
         <v>-0.501</v>
       </c>
     </row>
@@ -4675,81 +4683,81 @@
         <v>18</v>
       </c>
       <c r="C73" s="7">
-        <f t="shared" ref="C73:H73" si="53">SUM(C64:C72)/COUNT(C64:C72)</f>
+        <f t="shared" ref="C73:H73" si="73">SUM(C64:C72)/COUNT(C64:C72)</f>
         <v>0.17055555555555557</v>
       </c>
       <c r="D73" s="7">
-        <f t="shared" si="53"/>
+        <f t="shared" si="73"/>
         <v>0.60599999999999998</v>
       </c>
       <c r="E73" s="7">
-        <f t="shared" si="53"/>
+        <f t="shared" si="73"/>
         <v>0.24388888888888893</v>
       </c>
       <c r="F73" s="7">
-        <f t="shared" si="53"/>
+        <f t="shared" si="73"/>
         <v>0.64822222222222214</v>
       </c>
       <c r="G73" s="7">
-        <f t="shared" si="53"/>
+        <f t="shared" si="73"/>
         <v>0.66355555555555557</v>
       </c>
       <c r="H73" s="7">
-        <f t="shared" si="53"/>
+        <f t="shared" si="73"/>
         <v>0.1331111111111111</v>
       </c>
       <c r="J73" s="3" t="s">
         <v>18</v>
       </c>
       <c r="K73" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="59"/>
         <v>0.24866666666666665</v>
       </c>
       <c r="L73" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="60"/>
         <v>-4.3444444444444508E-2</v>
       </c>
       <c r="M73" s="2">
-        <f t="shared" si="49"/>
+        <f t="shared" si="61"/>
         <v>9.3777777777777793E-2</v>
       </c>
       <c r="N73" s="2">
-        <f t="shared" si="50"/>
+        <f t="shared" si="62"/>
         <v>0.10044444444444456</v>
       </c>
       <c r="O73" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="63"/>
         <v>0.11755555555555552</v>
       </c>
       <c r="P73" s="2">
-        <f t="shared" si="52"/>
+        <f t="shared" si="64"/>
         <v>0.16244444444444447</v>
       </c>
       <c r="R73" s="3" t="s">
         <v>18</v>
       </c>
       <c r="S73" s="2">
-        <f>C73-K$45</f>
+        <f t="shared" ref="S73:X73" si="74">C73-K$45</f>
         <v>7.8111111111111131E-2</v>
       </c>
       <c r="T73" s="2">
-        <f>D73-L$45</f>
+        <f t="shared" si="74"/>
         <v>2.011111111111108E-2</v>
       </c>
       <c r="U73" s="2">
-        <f>E73-M$45</f>
+        <f t="shared" si="74"/>
         <v>9.911111111111115E-2</v>
       </c>
       <c r="V73" s="2">
-        <f>F73-N$45</f>
+        <f t="shared" si="74"/>
         <v>0.27622222222222209</v>
       </c>
       <c r="W73" s="2">
-        <f>G73-O$45</f>
+        <f t="shared" si="74"/>
         <v>0.35788888888888892</v>
       </c>
       <c r="X73" s="2">
-        <f>H73-P$45</f>
+        <f t="shared" si="74"/>
         <v>9.1222222222222205E-2</v>
       </c>
     </row>
@@ -4785,54 +4793,54 @@
         <v>19</v>
       </c>
       <c r="K74" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="59"/>
         <v>0.22761846153846155</v>
       </c>
       <c r="L74" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="60"/>
         <v>-4.1176755447941971E-2</v>
       </c>
       <c r="M74" s="2">
-        <f t="shared" si="49"/>
+        <f t="shared" si="61"/>
         <v>6.9699757869249396E-2</v>
       </c>
       <c r="N74" s="2">
-        <f t="shared" si="50"/>
+        <f t="shared" si="62"/>
         <v>7.6876513317191364E-2</v>
       </c>
       <c r="O74" s="2">
-        <f t="shared" si="51"/>
+        <f t="shared" si="63"/>
         <v>7.1845036319612698E-2</v>
       </c>
       <c r="P74" s="2">
-        <f t="shared" si="52"/>
+        <f t="shared" si="64"/>
         <v>0.12975302663438254</v>
       </c>
       <c r="R74" s="3" t="s">
         <v>19</v>
       </c>
       <c r="S74" s="2">
-        <f>C74-K$46</f>
+        <f t="shared" ref="S74:X74" si="75">C74-K$46</f>
         <v>9.5956937977276974E-2</v>
       </c>
       <c r="T74" s="2">
-        <f>D74-L$46</f>
+        <f t="shared" si="75"/>
         <v>4.3496368038740796E-2</v>
       </c>
       <c r="U74" s="2">
-        <f>E74-M$46</f>
+        <f t="shared" si="75"/>
         <v>8.3845036319612598E-2</v>
       </c>
       <c r="V74" s="2">
-        <f>F74-N$46</f>
+        <f t="shared" si="75"/>
         <v>0.22752542372881346</v>
       </c>
       <c r="W74" s="2">
-        <f>G74-O$46</f>
+        <f t="shared" si="75"/>
         <v>0.34651815980629525</v>
       </c>
       <c r="X74" s="2">
-        <f>H74-P$46</f>
+        <f t="shared" si="75"/>
         <v>0.11672881355932205</v>
       </c>
     </row>
@@ -4845,6 +4853,8 @@
       <c r="B77" t="s">
         <v>29</v>
       </c>
+      <c r="N77" s="14"/>
+      <c r="O77" s="14"/>
     </row>
     <row r="78" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B78" s="4" t="s">
@@ -4883,6 +4893,12 @@
       <c r="M78" s="13" t="s">
         <v>17</v>
       </c>
+      <c r="N78" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="O78" s="15" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="79" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B79" s="3" t="s">
@@ -4929,13 +4945,21 @@
         <f>((D79*G79)-(E79*F79))/SQRT((D79+E79)*(D79+F79)*(G79+E79)*(G79+F79))</f>
         <v>0.73029674334022143</v>
       </c>
+      <c r="N79">
+        <f>IF(H79&gt;=I79,SQRT((E79+G79)*(D79+E79))/SQRT((F79+G79)*(D79+F79)),SQRT((F79+G79)*(D79+F79))/SQRT((E79+G79)*(D79+E79)))</f>
+        <v>0.73029674334022154</v>
+      </c>
+      <c r="O79">
+        <f>M79/N79</f>
+        <v>0.99999999999999989</v>
+      </c>
     </row>
     <row r="80" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B80" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C80">
-        <f t="shared" ref="C80:C87" si="54">D80+F80</f>
+        <f t="shared" ref="C80:C87" si="76">D80+F80</f>
         <v>5</v>
       </c>
       <c r="D80">
@@ -4960,28 +4984,36 @@
         <v>1</v>
       </c>
       <c r="J80" s="2">
-        <f t="shared" ref="J80:J87" si="55">2*H80*I80/(H80+I80)</f>
+        <f t="shared" ref="J80:J87" si="77">2*H80*I80/(H80+I80)</f>
         <v>1</v>
       </c>
       <c r="K80">
-        <f t="shared" ref="K80:K87" si="56">(D80+G80)/SUM(D80:G80)</f>
+        <f t="shared" ref="K80:K87" si="78">(D80+G80)/SUM(D80:G80)</f>
         <v>1</v>
       </c>
       <c r="L80">
-        <f t="shared" ref="L80:L87" si="57">G80/(G80+E80)</f>
+        <f t="shared" ref="L80:L87" si="79">G80/(G80+E80)</f>
         <v>1</v>
       </c>
       <c r="M80">
-        <f t="shared" ref="M80:M87" si="58">((D80*G80)-(E80*F80))/SQRT((D80+E80)*(D80+F80)*(G80+E80)*(G80+F80))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" ref="M80:M87" si="80">((D80*G80)-(E80*F80))/SQRT((D80+E80)*(D80+F80)*(G80+E80)*(G80+F80))</f>
+        <v>1</v>
+      </c>
+      <c r="N80">
+        <f t="shared" ref="N80:N87" si="81">IF(H80&gt;=I80,SQRT((E80+G80)*(D80+E80))/SQRT((F80+G80)*(D80+F80)),SQRT((F80+G80)*(D80+F80))/SQRT((E80+G80)*(D80+E80)))</f>
+        <v>1</v>
+      </c>
+      <c r="O80">
+        <f t="shared" ref="O80:O87" si="82">M80/N80</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B81" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C81">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>5</v>
       </c>
       <c r="D81">
@@ -5006,28 +5038,36 @@
         <v>1</v>
       </c>
       <c r="J81" s="2">
-        <f t="shared" si="55"/>
+        <f t="shared" si="77"/>
         <v>0.90909090909090906</v>
       </c>
       <c r="K81">
-        <f t="shared" si="56"/>
+        <f t="shared" si="78"/>
         <v>0.91666666666666663</v>
       </c>
       <c r="L81">
-        <f t="shared" si="57"/>
+        <f t="shared" si="79"/>
         <v>0.8571428571428571</v>
       </c>
       <c r="M81">
-        <f t="shared" si="58"/>
+        <f t="shared" si="80"/>
         <v>0.84515425472851657</v>
       </c>
-    </row>
-    <row r="82" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N81">
+        <f t="shared" si="81"/>
+        <v>0.84515425472851657</v>
+      </c>
+      <c r="O81">
+        <f t="shared" si="82"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B82" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C82">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="D82">
@@ -5047,12 +5087,12 @@
       <c r="I82" s="2"/>
       <c r="J82" s="2"/>
     </row>
-    <row r="83" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B83" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C83">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="D83">
@@ -5077,28 +5117,36 @@
         <v>1</v>
       </c>
       <c r="J83" s="2">
-        <f t="shared" si="55"/>
+        <f t="shared" si="77"/>
         <v>1</v>
       </c>
       <c r="K83">
-        <f t="shared" si="56"/>
+        <f t="shared" si="78"/>
         <v>1</v>
       </c>
       <c r="L83">
-        <f t="shared" si="57"/>
+        <f t="shared" si="79"/>
         <v>1</v>
       </c>
       <c r="M83">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="80"/>
+        <v>1</v>
+      </c>
+      <c r="N83">
+        <f t="shared" si="81"/>
+        <v>1</v>
+      </c>
+      <c r="O83">
+        <f t="shared" si="82"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B84" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C84">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="D84">
@@ -5123,28 +5171,36 @@
         <v>1</v>
       </c>
       <c r="J84" s="2">
-        <f t="shared" si="55"/>
+        <f t="shared" si="77"/>
         <v>1</v>
       </c>
       <c r="K84">
-        <f t="shared" si="56"/>
+        <f t="shared" si="78"/>
         <v>1</v>
       </c>
       <c r="L84">
-        <f t="shared" si="57"/>
+        <f t="shared" si="79"/>
         <v>1</v>
       </c>
       <c r="M84">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="80"/>
+        <v>1</v>
+      </c>
+      <c r="N84">
+        <f t="shared" si="81"/>
+        <v>1</v>
+      </c>
+      <c r="O84">
+        <f t="shared" si="82"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B85" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C85">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>6</v>
       </c>
       <c r="D85">
@@ -5169,28 +5225,36 @@
         <v>0.5</v>
       </c>
       <c r="J85" s="2">
-        <f t="shared" si="55"/>
+        <f t="shared" si="77"/>
         <v>0.6</v>
       </c>
       <c r="K85">
-        <f t="shared" si="56"/>
+        <f t="shared" si="78"/>
         <v>0.69230769230769229</v>
       </c>
       <c r="L85">
-        <f t="shared" si="57"/>
+        <f t="shared" si="79"/>
         <v>0.8571428571428571</v>
       </c>
       <c r="M85">
-        <f t="shared" si="58"/>
+        <f t="shared" si="80"/>
         <v>0.38575837490522974</v>
       </c>
-    </row>
-    <row r="86" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N85">
+        <f t="shared" si="81"/>
+        <v>0.72008229982309557</v>
+      </c>
+      <c r="O85">
+        <f t="shared" si="82"/>
+        <v>0.5357142857142857</v>
+      </c>
+    </row>
+    <row r="86" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B86" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C86">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="D86">
@@ -5215,28 +5279,36 @@
         <v>1</v>
       </c>
       <c r="J86" s="9">
-        <f t="shared" si="55"/>
+        <f t="shared" si="77"/>
         <v>1</v>
       </c>
       <c r="K86">
-        <f t="shared" si="56"/>
+        <f t="shared" si="78"/>
         <v>1</v>
       </c>
       <c r="L86">
-        <f t="shared" si="57"/>
+        <f t="shared" si="79"/>
         <v>1</v>
       </c>
       <c r="M86">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="80"/>
+        <v>1</v>
+      </c>
+      <c r="N86">
+        <f t="shared" si="81"/>
+        <v>1</v>
+      </c>
+      <c r="O86">
+        <f t="shared" si="82"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B87" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C87" s="8">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>2</v>
       </c>
       <c r="D87" s="5">
@@ -5261,23 +5333,31 @@
         <v>1</v>
       </c>
       <c r="J87" s="10">
-        <f t="shared" si="55"/>
+        <f t="shared" si="77"/>
         <v>0.8</v>
       </c>
       <c r="K87" s="5">
-        <f t="shared" si="56"/>
+        <f t="shared" si="78"/>
         <v>0.8571428571428571</v>
       </c>
       <c r="L87" s="5">
-        <f t="shared" si="57"/>
+        <f t="shared" si="79"/>
         <v>0.8</v>
       </c>
       <c r="M87" s="5">
-        <f t="shared" si="58"/>
+        <f t="shared" si="80"/>
         <v>0.73029674334022143</v>
       </c>
-    </row>
-    <row r="88" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N87" s="5">
+        <f t="shared" si="81"/>
+        <v>0.73029674334022154</v>
+      </c>
+      <c r="O87" s="5">
+        <f t="shared" si="82"/>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="88" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B88" s="6" t="s">
         <v>18</v>
       </c>
@@ -5297,19 +5377,27 @@
         <v>0.88863636363636356</v>
       </c>
       <c r="K88" s="2">
-        <f t="shared" ref="K88:M88" si="59">SUM(K79:K87)/COUNT(K79:K87)</f>
+        <f t="shared" ref="K88:O88" si="83">SUM(K79:K87)/COUNT(K79:K87)</f>
         <v>0.91540750915750912</v>
       </c>
       <c r="L88" s="2">
-        <f t="shared" si="59"/>
+        <f t="shared" si="83"/>
         <v>0.93928571428571428</v>
       </c>
       <c r="M88" s="2">
-        <f t="shared" si="59"/>
+        <f t="shared" si="83"/>
         <v>0.83643826453927361</v>
       </c>
-    </row>
-    <row r="89" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N88" s="2">
+        <f t="shared" si="83"/>
+        <v>0.87822875515400689</v>
+      </c>
+      <c r="O88" s="2">
+        <f t="shared" si="83"/>
+        <v>0.9419642857142857</v>
+      </c>
+    </row>
+    <row r="89" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B89" s="3" t="s">
         <v>19</v>
       </c>
@@ -5317,28 +5405,36 @@
       <c r="E89" s="11"/>
       <c r="F89" s="11"/>
       <c r="H89" s="11">
-        <f>(($C79*H79)+($C80*H80)+($C81*H81)+($C82*H82)+($C83*H83)+($C84*H84)+($C85*H85)+($C86*H86)+($C87*H87))/SUM($C79:$C87)</f>
+        <f t="shared" ref="H89:O89" si="84">(($C79*H79)+($C80*H80)+($C81*H81)+($C82*H82)+($C83*H83)+($C84*H84)+($C85*H85)+($C86*H86)+($C87*H87))/SUM($C79:$C87)</f>
         <v>0.88888888888888884</v>
       </c>
       <c r="I89" s="11">
-        <f>(($C79*I79)+($C80*I80)+($C81*I81)+($C82*I82)+($C83*I83)+($C84*I84)+($C85*I85)+($C86*I86)+($C87*I87))/SUM($C79:$C87)</f>
+        <f t="shared" si="84"/>
         <v>0.81481481481481477</v>
       </c>
       <c r="J89" s="11">
-        <f>(($C79*J79)+($C80*J80)+($C81*J81)+($C82*J82)+($C83*J83)+($C84*J84)+($C85*J85)+($C86*J86)+($C87*J87))/SUM($C79:$C87)</f>
+        <f t="shared" si="84"/>
         <v>0.8350168350168351</v>
       </c>
       <c r="K89" s="11">
-        <f>(($C79*K79)+($C80*K80)+($C81*K81)+($C82*K82)+($C83*K83)+($C84*K84)+($C85*K85)+($C86*K86)+($C87*K87))/SUM($C79:$C87)</f>
+        <f t="shared" si="84"/>
         <v>0.87386379053045715</v>
       </c>
       <c r="L89" s="11">
-        <f>(($C79*L79)+($C80*L80)+($C81*L81)+($C82*L82)+($C83*L83)+($C84*L84)+($C85*L85)+($C86*L86)+($C87*L87))/SUM($C79:$C87)</f>
+        <f t="shared" si="84"/>
         <v>0.92698412698412702</v>
       </c>
       <c r="M89" s="11">
-        <f>(($C79*M79)+($C80*M80)+($C81*M81)+($C82*M82)+($C83*M83)+($C84*M84)+($C85*M85)+($C86*M86)+($C87*M87))/SUM($C79:$C87)</f>
+        <f t="shared" si="84"/>
         <v>0.75491464702947164</v>
+      </c>
+      <c r="N89" s="11">
+        <f t="shared" si="84"/>
+        <v>0.82920885256677512</v>
+      </c>
+      <c r="O89" s="11">
+        <f t="shared" si="84"/>
+        <v>0.89682539682539686</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update results for UME
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -559,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:X89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="P82" sqref="P82"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="R82" sqref="R82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4906,28 +4906,28 @@
       </c>
       <c r="C79">
         <f>D79+F79</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D79">
         <v>4</v>
       </c>
       <c r="E79">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F79">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G79">
         <f>Info!C2-C79</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H79" s="2">
         <f>D79/(D79+E79)</f>
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="I79" s="2">
         <f>D79/(D79+F79)</f>
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="J79" s="2">
         <f>2*H79*I79/(H79+I79)</f>
@@ -4935,19 +4935,19 @@
       </c>
       <c r="K79">
         <f>(D79+G79)/SUM(D79:G79)</f>
-        <v>0.8571428571428571</v>
+        <v>0.875</v>
       </c>
       <c r="L79">
         <f>G79/(G79+E79)</f>
-        <v>1</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="M79">
         <f>((D79*G79)-(E79*F79))/SQRT((D79+E79)*(D79+F79)*(G79+E79)*(G79+F79))</f>
-        <v>0.73029674334022143</v>
+        <v>0.7453559924999299</v>
       </c>
       <c r="N79">
         <f>IF(H79&gt;=I79,SQRT((E79+G79)*(D79+E79))/SQRT((F79+G79)*(D79+F79)),SQRT((F79+G79)*(D79+F79))/SQRT((E79+G79)*(D79+E79)))</f>
-        <v>0.73029674334022154</v>
+        <v>0.74535599249993001</v>
       </c>
       <c r="O79">
         <f>M79/N79</f>
@@ -5014,28 +5014,28 @@
       </c>
       <c r="C81">
         <f t="shared" si="76"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D81">
         <v>5</v>
       </c>
       <c r="E81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G81">
         <f>Info!C4-C81</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H81" s="2">
         <f>D81/(D81+E81)</f>
-        <v>0.83333333333333337</v>
+        <v>1</v>
       </c>
       <c r="I81" s="2">
         <f>D81/(D81+F81)</f>
-        <v>1</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="J81" s="2">
         <f t="shared" si="77"/>
@@ -5043,19 +5043,19 @@
       </c>
       <c r="K81">
         <f t="shared" si="78"/>
-        <v>0.91666666666666663</v>
+        <v>0.90909090909090906</v>
       </c>
       <c r="L81">
         <f t="shared" si="79"/>
-        <v>0.8571428571428571</v>
+        <v>1</v>
       </c>
       <c r="M81">
         <f t="shared" si="80"/>
-        <v>0.84515425472851657</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="N81">
         <f t="shared" si="81"/>
-        <v>0.84515425472851657</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="O81">
         <f t="shared" si="82"/>
@@ -5086,6 +5086,14 @@
       <c r="H82" s="2"/>
       <c r="I82" s="2"/>
       <c r="J82" s="2"/>
+      <c r="K82">
+        <f t="shared" si="78"/>
+        <v>1</v>
+      </c>
+      <c r="L82">
+        <f t="shared" si="79"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="83" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B83" s="3" t="s">
@@ -5201,28 +5209,28 @@
       </c>
       <c r="C85">
         <f t="shared" si="76"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D85">
         <v>3</v>
       </c>
       <c r="E85">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F85">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G85">
         <f>Info!C8-C85</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H85" s="2">
         <f>D85/(D85+E85)</f>
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="I85" s="2">
         <f>D85/(D85+F85)</f>
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="J85" s="2">
         <f t="shared" si="77"/>
@@ -5230,23 +5238,23 @@
       </c>
       <c r="K85">
         <f t="shared" si="78"/>
-        <v>0.69230769230769229</v>
+        <v>0.73333333333333328</v>
       </c>
       <c r="L85">
         <f t="shared" si="79"/>
-        <v>0.8571428571428571</v>
+        <v>0.72727272727272729</v>
       </c>
       <c r="M85">
         <f t="shared" si="80"/>
-        <v>0.38575837490522974</v>
+        <v>0.43082021842766455</v>
       </c>
       <c r="N85">
         <f t="shared" si="81"/>
-        <v>0.72008229982309557</v>
+        <v>0.7385489458759964</v>
       </c>
       <c r="O85">
         <f t="shared" si="82"/>
-        <v>0.5357142857142857</v>
+        <v>0.58333333333333326</v>
       </c>
     </row>
     <row r="86" spans="2:15" x14ac:dyDescent="0.25">
@@ -5309,28 +5317,28 @@
       </c>
       <c r="C87" s="8">
         <f t="shared" si="76"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D87" s="5">
         <v>2</v>
       </c>
       <c r="E87" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F87" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G87" s="5">
         <f>Info!C10-C87</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H87" s="10">
         <f>D87/(D87+E87)</f>
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="I87" s="10">
         <f>D87/(D87+F87)</f>
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="J87" s="10">
         <f t="shared" si="77"/>
@@ -5338,23 +5346,23 @@
       </c>
       <c r="K87" s="5">
         <f t="shared" si="78"/>
-        <v>0.8571428571428571</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="L87" s="5">
         <f t="shared" si="79"/>
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="M87" s="5">
         <f t="shared" si="80"/>
-        <v>0.73029674334022143</v>
+        <v>0.70710678118654757</v>
       </c>
       <c r="N87" s="5">
         <f t="shared" si="81"/>
-        <v>0.73029674334022154</v>
+        <v>0.70710678118654746</v>
       </c>
       <c r="O87" s="5">
         <f t="shared" si="82"/>
-        <v>0.99999999999999989</v>
+        <v>1.0000000000000002</v>
       </c>
     </row>
     <row r="88" spans="2:15" x14ac:dyDescent="0.25">
@@ -5366,11 +5374,11 @@
       <c r="F88" s="2"/>
       <c r="H88" s="2">
         <f>SUM(H79:H87)/COUNT(H79:H87)</f>
-        <v>0.90625000000000011</v>
+        <v>0.89583333333333326</v>
       </c>
       <c r="I88" s="2">
         <f>SUM(I79:I87)/COUNT(I79:I87)</f>
-        <v>0.89583333333333326</v>
+        <v>0.90625000000000011</v>
       </c>
       <c r="J88" s="2">
         <f>SUM(J79:J87)/COUNT(J79:J87)</f>
@@ -5378,23 +5386,23 @@
       </c>
       <c r="K88" s="2">
         <f t="shared" ref="K88:O88" si="83">SUM(K79:K87)/COUNT(K79:K87)</f>
-        <v>0.91540750915750912</v>
+        <v>0.92786195286195294</v>
       </c>
       <c r="L88" s="2">
         <f t="shared" si="83"/>
-        <v>0.93928571428571428</v>
+        <v>0.95117845117845135</v>
       </c>
       <c r="M88" s="2">
         <f t="shared" si="83"/>
-        <v>0.83643826453927361</v>
+        <v>0.83957704068093442</v>
       </c>
       <c r="N88" s="2">
         <f t="shared" si="83"/>
-        <v>0.87822875515400689</v>
+        <v>0.87804313161197589</v>
       </c>
       <c r="O88" s="2">
         <f t="shared" si="83"/>
-        <v>0.9419642857142857</v>
+        <v>0.94791666666666663</v>
       </c>
     </row>
     <row r="89" spans="2:15" x14ac:dyDescent="0.25">
@@ -5406,35 +5414,35 @@
       <c r="F89" s="11"/>
       <c r="H89" s="11">
         <f t="shared" ref="H89:O89" si="84">(($C79*H79)+($C80*H80)+($C81*H81)+($C82*H82)+($C83*H83)+($C84*H84)+($C85*H85)+($C86*H86)+($C87*H87))/SUM($C79:$C87)</f>
-        <v>0.88888888888888884</v>
+        <v>0.86666666666666659</v>
       </c>
       <c r="I89" s="11">
         <f t="shared" si="84"/>
-        <v>0.81481481481481477</v>
+        <v>0.88</v>
       </c>
       <c r="J89" s="11">
         <f t="shared" si="84"/>
-        <v>0.8350168350168351</v>
+        <v>0.85818181818181816</v>
       </c>
       <c r="K89" s="11">
         <f t="shared" si="84"/>
-        <v>0.87386379053045715</v>
+        <v>0.89551515151515149</v>
       </c>
       <c r="L89" s="11">
         <f t="shared" si="84"/>
-        <v>0.92698412698412702</v>
+        <v>0.9296969696969698</v>
       </c>
       <c r="M89" s="11">
         <f t="shared" si="84"/>
-        <v>0.75491464702947164</v>
+        <v>0.79304100749080075</v>
       </c>
       <c r="N89" s="11">
         <f t="shared" si="84"/>
-        <v>0.82920885256677512</v>
+        <v>0.84227760388253403</v>
       </c>
       <c r="O89" s="11">
         <f t="shared" si="84"/>
-        <v>0.89682539682539686</v>
+        <v>0.93333333333333324</v>
       </c>
     </row>
   </sheetData>

</xml_diff>